<commit_message>
Changed Tab DRGv2 to DRGs
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-Flat-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-Flat-template.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Policies" sheetId="4" r:id="rId4"/>
     <sheet name="Tags" sheetId="22" r:id="rId5"/>
     <sheet name="VCNs" sheetId="5" r:id="rId6"/>
-    <sheet name="DRGv2" sheetId="32" r:id="rId7"/>
+    <sheet name="DRGs" sheetId="32" r:id="rId7"/>
     <sheet name="VCN Info" sheetId="6" r:id="rId8"/>
     <sheet name="DHCP" sheetId="7" r:id="rId9"/>
     <sheet name="Subnets" sheetId="8" r:id="rId10"/>
@@ -6585,77 +6585,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Automation Toolkit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>release version-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">v8.0
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Added new sheets - DRGv2 and DRGRouteRulesinOCI
-</t>
-    </r>
-  </si>
-  <si>
     <t>DRG Name</t>
   </si>
   <si>
@@ -6669,12 +6598,6 @@
   </si>
   <si>
     <t>Import DRG Route Distribution Statements</t>
-  </si>
-  <si>
-    <t>DRG Route Rules will be exported here
-"Defined Tags" - Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
-                                Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
-                                Example: Operations.CostCenter=01;Users.Name=user01</t>
   </si>
   <si>
     <t>Next Hop Attachment</t>
@@ -6713,6 +6636,83 @@
   </si>
   <si>
     <t>DRG_ATTACHMENT_TYPE::VCN::1</t>
+  </si>
+  <si>
+    <t>DRG Route Rules will be exported here for DRGv2.
+"Defined Tags" - Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
+                                Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
+                                Example: Operations.CostCenter=01;Users.Name=user01</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Automation Toolkit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>release version-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">v8.0
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Added new sheets - DRGs and DRGRouteRulesinOCI
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -9420,7 +9420,7 @@
     <row r="1" spans="1:1" ht="15" thickBot="1"/>
     <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1">
       <c r="A2" s="61" t="s">
-        <v>878</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>
@@ -10015,8 +10015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10037,7 +10037,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1">
       <c r="A1" s="92" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="B1" s="92"/>
       <c r="C1" s="92"/>
@@ -10057,25 +10057,25 @@
         <v>6</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D2" s="32" t="s">
+        <v>880</v>
+      </c>
+      <c r="E2" s="33" t="s">
         <v>881</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>882</v>
       </c>
       <c r="F2" s="32" t="s">
         <v>61</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>63</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="J2" s="32" t="s">
         <v>435</v>
@@ -20116,7 +20116,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="F3" s="40" t="s">
         <v>21</v>
@@ -20291,7 +20291,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="205" customHeight="1">
       <c r="A1" s="92" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -20308,19 +20308,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="89" t="s">
+        <v>878</v>
+      </c>
+      <c r="D2" s="89" t="s">
         <v>879</v>
       </c>
-      <c r="D2" s="89" t="s">
+      <c r="E2" s="89" t="s">
         <v>880</v>
       </c>
-      <c r="E2" s="89" t="s">
+      <c r="F2" s="90" t="s">
         <v>881</v>
       </c>
-      <c r="F2" s="90" t="s">
+      <c r="G2" s="91" t="s">
         <v>882</v>
-      </c>
-      <c r="G2" s="91" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" customHeight="1">
@@ -20331,19 +20331,19 @@
         <v>355</v>
       </c>
       <c r="C3" s="38" t="s">
+        <v>886</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>887</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>888</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="F3" s="38" t="s">
         <v>889</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="G3" s="38" t="s">
         <v>890</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>891</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="94.5" customHeight="1">

</xml_diff>

<commit_message>
correted templates, modified export_network_nonGreenField.py
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-Flat-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-Flat-template.xlsx
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="894">
   <si>
     <t>Region</t>
   </si>
@@ -6699,21 +6699,28 @@
   </si>
   <si>
     <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;).
-Columns Region, Compartment Name, DRG Name, Attached To are mandatory.
-Leave columns DRG RT Name,  Import DRG Route Distribution Name and Import DRG Route Distribution Statements empty to use Autogenerated ones.
-Compartment Name specifies compartment where DRG has to be created. DRG Attachment is created in same compartment as target VCN, IPSEC or RPC by default.
-Leave column Attached To empty if only DRG Route Table or DRG Import Route Distribution is to be created for the DRG.
+- Columns Region, Compartment Name, DRG Name are mandatory.
+- Leave columns DRG RT Name,  Import DRG Route Distribution Name and Import DRG   Route Distribution Statements empty to use Autogenerated ones.
+- Compartment Name specifies compartment where DRG has to be created. DRG Attachment is created in same compartment as target VCN, IPSEC or RPC by default.
+- Leave column Attached To empty if only DRG Route Table or DRG Import Route Distribution is to be created for the DRG.
+"Defined Tags" - Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
+Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
+Example: Operations.CostCenter=01;Users.Name=user01
+</t>
+  </si>
+  <si>
+    <t>"Attached To" - Valid format:
+VCN::&lt;vcn_name&gt;
+IPSEC_TUNNEL::&lt;OCID&gt;
+VIRTUAL_CIRCUIT::&lt;OCID&gt;
+REMOTE_PEERING_CONNECTION::&lt;OCID&gt;
 "Import DRG Route Distribution Statements" - Valid format: &lt;matchtype&gt;::&lt;type|ocid&gt;::&lt;priority&gt;  Multiple statements are seperated by newline(\n is not supported)
  eg: ALL::::1
        DRG_ATTACHMENT_TYPE::VCN::2
        DRG_ATTACHMENT_TYPE::IPSEC_TUNNEL::2
        DRG_ATTACHMENT_TYPE::REMOTE_PEERING_CONNECTION::2
        DRG_ATTACHMENT_TYPE::VIRTUAL_CIRCUIT::2
-       DRG_ATTACHMENT_ID::&lt;OCID&gt;::3
-"Defined Tags" - Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
-                                Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
-                                Example: Operations.CostCenter=01;Users.Name=user01
-</t>
+       DRG_ATTACHMENT_ID::&lt;OCID&gt;::3</t>
   </si>
 </sst>
 </file>
@@ -7213,7 +7220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7443,8 +7450,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -9470,18 +9475,18 @@
       <c r="F1" s="94"/>
       <c r="G1" s="94"/>
       <c r="H1" s="95"/>
-      <c r="I1" s="101" t="s">
+      <c r="I1" s="99" t="s">
         <v>451</v>
       </c>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
     </row>
     <row r="2" spans="1:18" s="47" customFormat="1" ht="59.5" customHeight="1">
       <c r="A2" s="11" t="s">
@@ -12889,16 +12894,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="117" customHeight="1">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="100" t="s">
         <v>877</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="104"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="102"/>
       <c r="I1" s="93" t="s">
         <v>586</v>
       </c>
@@ -13351,27 +13356,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="110.5" customHeight="1">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="103" t="s">
         <v>468</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="108" t="s">
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="106" t="s">
         <v>462</v>
       </c>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="106"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="51.75" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -14501,15 +14506,15 @@
       <c r="J1" s="96" t="s">
         <v>470</v>
       </c>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="109"/>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="109"/>
-      <c r="R1" s="109"/>
-      <c r="S1" s="110"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="108"/>
     </row>
     <row r="2" spans="1:19" ht="58.75" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -15174,14 +15179,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="47" customFormat="1" ht="44.5" customHeight="1">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="109" t="s">
         <v>446</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="113"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="111"/>
     </row>
     <row r="2" spans="1:6" ht="14.5" customHeight="1">
       <c r="A2" s="21" t="s">
@@ -15551,17 +15556,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="114" customHeight="1">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="112" t="s">
         <v>817</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="8" t="s">
@@ -20028,7 +20033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -20274,7 +20279,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -20283,23 +20288,25 @@
     <col min="2" max="2" width="18" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.81640625" style="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1796875" style="39" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.08984375" style="39" customWidth="1"/>
     <col min="6" max="6" width="30.81640625" style="39" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.08984375" style="39" customWidth="1"/>
     <col min="8" max="18" width="8.7265625" style="39" customWidth="1"/>
     <col min="19" max="16384" width="8.7265625" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="205" customHeight="1">
-      <c r="A1" s="92" t="s">
+    <row r="1" spans="1:7" ht="221" customHeight="1">
+      <c r="A1" s="93" t="s">
         <v>892</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="100"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="93" t="s">
+        <v>893</v>
+      </c>
+      <c r="G1" s="94"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="89" t="s">
@@ -20591,8 +20598,9 @@
       <c r="G30" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
updated commonTools.py to do File handling updated templates as per CIS LZ v2
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-Flat-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-Flat-template.xlsx
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="912">
   <si>
     <t>Region</t>
   </si>
@@ -5148,9 +5148,6 @@
     <t>Allow group AppDevAdmins to read instance-images in tenancy</t>
   </si>
   <si>
-    <t>Allow group AppDevAdmins to manage repos in tenancy</t>
-  </si>
-  <si>
     <t>Allow group AppDevAdmins to manage orm-stacks in compartment AppDev</t>
   </si>
   <si>
@@ -5313,21 +5310,9 @@
     <t>Policy allowing IAMAdmins group to manage IAM resources in tenancy, except changing Administrators group assignments.</t>
   </si>
   <si>
-    <t>Allow group IAMAdmins to manage users in tenancy</t>
-  </si>
-  <si>
     <t>Allow group IAMAdmins to inspect groups in tenancy</t>
   </si>
   <si>
-    <t>Allow group IAMAdmins to manage groups in tenancy where target.group.name != 'Administrators'</t>
-  </si>
-  <si>
-    <t>Allow group IAMAdmins to inspect policies in tenancy</t>
-  </si>
-  <si>
-    <t>Allow group IAMAdmins to manage policies in tenancy where target.policy.name != 'Tenant Admin Policy'</t>
-  </si>
-  <si>
     <t>Allow group IAMAdmins to manage dynamic-groups in tenancy</t>
   </si>
   <si>
@@ -5337,9 +5322,6 @@
     <t>Allow group IAMAdmins to manage authentication-policies in tenancy</t>
   </si>
   <si>
-    <t>Allow group IAMAdmins to manage identity-providers in tenancy</t>
-  </si>
-  <si>
     <t>Allow group IAMAdmins to manage network-sources in tenancy</t>
   </si>
   <si>
@@ -5349,9 +5331,6 @@
     <t>Allow group IAMAdmins to manage tag-namespaces in tenancy</t>
   </si>
   <si>
-    <t>Allow group IAMAdmins to manage credentials in tenancy</t>
-  </si>
-  <si>
     <t>Allow group IAMAdmins to manage orm-stacks in tenancy</t>
   </si>
   <si>
@@ -5406,12 +5385,6 @@
     <t>Allow group SecurityAdmins to manage instance-family in compartment Security</t>
   </si>
   <si>
-    <t>Allow group SecurityAdmins to manage policies in tenancy where all {target.policy.name != 'Tenant Admin Policy', target.policy.name != 'IAMAdmins-Policy'}</t>
-  </si>
-  <si>
-    <t>Allow group SecurityAdmins to manage policies in compartment Security</t>
-  </si>
-  <si>
     <t>Allow group SecurityAdmins to manage vaults in compartment Security</t>
   </si>
   <si>
@@ -5424,9 +5397,6 @@
     <t>Allow group SecurityAdmins to manage logging-family in compartment Security</t>
   </si>
   <si>
-    <t>Allow group SecurityAdmins to manage cloudevents-rules in compartment Security</t>
-  </si>
-  <si>
     <t>Allow group SecurityAdmins to manage serviceconnectors in compartment Security</t>
   </si>
   <si>
@@ -5445,18 +5415,6 @@
     <t>Allow group SecurityAdmins to manage security-zone in compartment Security</t>
   </si>
   <si>
-    <t>Allow group SecurityAdmins to read virtual-network-family in compartment Network</t>
-  </si>
-  <si>
-    <t>Allow group SecurityAdmins to use subnets in compartment Network</t>
-  </si>
-  <si>
-    <t>Allow group SecurityAdmins to use network-security-groups in compartment Network</t>
-  </si>
-  <si>
-    <t>Allow group SecurityAdmins to use vnics in compartment Network</t>
-  </si>
-  <si>
     <t>Allow group SecurityAdmins to manage tag-namespaces in tenancy</t>
   </si>
   <si>
@@ -5493,15 +5451,6 @@
     <t>Allow group SecurityAdmins to manage orm-config-source-providers in compartment Security</t>
   </si>
   <si>
-    <t>CrossTenancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows Security Auditors to Read Stuff in my tenancy </t>
-  </si>
-  <si>
-    <t>Endorse group Administrators to read all-resources in any-tenancy</t>
-  </si>
-  <si>
     <t>10.110.2.0/24</t>
   </si>
   <si>
@@ -5644,9 +5593,6 @@
   </si>
   <si>
     <t>Allow Group DatabaseAdmins to read audit-events in compartment Database</t>
-  </si>
-  <si>
-    <t>Allow Group IAMAdmins to read audit-events in tenancy</t>
   </si>
   <si>
     <t>Allow Group NetworkAdmins to read audit-events in compartment Network</t>
@@ -6718,6 +6664,114 @@
        DRG_ATTACHMENT_TYPE::REMOTE_PEERING_CONNECTION::2
        DRG_ATTACHMENT_TYPE::VIRTUAL_CIRCUIT::2
        DRG_ATTACHMENT_ID::&lt;OCID&gt;::3</t>
+  </si>
+  <si>
+    <t>Allow group AnnouncementReaders to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>Allow Group Auditors to read users in tenancy</t>
+  </si>
+  <si>
+    <t>Allow Group Auditors to read vss-family in tenancy</t>
+  </si>
+  <si>
+    <t>CredAdmins</t>
+  </si>
+  <si>
+    <t>Group responsible for managing users credentials in the tenancy.</t>
+  </si>
+  <si>
+    <t>CredentialAdmins-Policy</t>
+  </si>
+  <si>
+    <t>Policy for Credential Admins Group</t>
+  </si>
+  <si>
+    <t>Allow group CredAdmins to inspect users in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group CredAdmins to inspect groups in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group CredAdmins to manage users in tenancy  where any {request.operation = 'ListApiKeys',request.operation = 'ListAuthTokens',request.operation = 'ListCustomerSecretKeys',request.operation = 'UploadApiKey',request.operation = 'DeleteApiKey',request.operation = 'UpdateAuthToken',request.operation = 'CreateAuthToken',request.operation = 'DeleteAuthToken',request.operation = 'CreateSecretKey',request.operation = 'UpdateCustomerSecretKey',request.operation = 'DeleteCustomerSecretKey',request.operation = 'UpdateUserCapabilities'}</t>
+  </si>
+  <si>
+    <t>Allow group CredAdmins to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group AppDevAdmins to manage instance-images in compartment Security</t>
+  </si>
+  <si>
+    <t>Allow group AppDevAdmins to manage repos in compartment AppDev</t>
+  </si>
+  <si>
+    <t>Allow group AppDevAdmins to read repos in tenancy</t>
+  </si>
+  <si>
+    <t>Allow Group AppDevAdmins to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group AppDevAdmins to read vss-family in compartment Security</t>
+  </si>
+  <si>
+    <t>Allow Group DatabaseAdmins to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group IAMAdmins to manage policies in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group IAMAdmins to inspect users in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group IAMAdmins to manage groups in tenancy where all {target.group.name != 'Administrators', target.group.name != 'CredAdmins'}</t>
+  </si>
+  <si>
+    <t>Allow group IAMAdmins to inspect identity-providers in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group IAMAdmins to manage identity-providers in tenancy where any {request.operation = 'AddIdpGroupMapping', request.operation = 'DeleteIdpGroupMapping'}</t>
+  </si>
+  <si>
+    <t>Allow group IAMAdmins to manage quota in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group IAMAdmins to read audit-events in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group IAMAdmins to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group NetworkAdmins to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group SecurityAdmins to manage repos in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group SecurityAdmins to manage cloudevents-rules in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group SecurityAdmins to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>Allow group SecurityAdmins to manage vss-family in compartment Security</t>
+  </si>
+  <si>
+    <t>Allow Group NetworkAdmins to read vss-family in compartment Security</t>
+  </si>
+  <si>
+    <t>Allow group DatabaseAdmins to read vss-family in compartment Database</t>
+  </si>
+  <si>
+    <t>Allow group SecurityAdmins to read virtual-network-family in compartment Network</t>
+  </si>
+  <si>
+    <t>Allow group SecurityAdmins to use subnets in compartment Network</t>
+  </si>
+  <si>
+    <t>Allow group SecurityAdmins to use network-security-groups in compartment Network</t>
+  </si>
+  <si>
+    <t>Allow group SecurityAdmins to use vnics in compartment Network</t>
   </si>
 </sst>
 </file>
@@ -7217,7 +7271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7424,6 +7478,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9423,7 +9483,7 @@
     <row r="1" spans="1:1" ht="15" thickBot="1"/>
     <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1">
       <c r="A2" s="61" t="s">
-        <v>891</v>
+        <v>873</v>
       </c>
     </row>
   </sheetData>
@@ -9462,28 +9522,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="173.5" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>444</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="99" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="101" t="s">
         <v>451</v>
       </c>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
+      <c r="P1" s="101"/>
+      <c r="Q1" s="101"/>
+      <c r="R1" s="101"/>
     </row>
     <row r="2" spans="1:18" s="47" customFormat="1" ht="59.5" customHeight="1">
       <c r="A2" s="11" t="s">
@@ -9549,10 +9609,10 @@
         <v>355</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>768</v>
+        <v>751</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>53</v>
@@ -9561,7 +9621,7 @@
         <v>54</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>749</v>
+        <v>732</v>
       </c>
       <c r="H3" s="40" t="s">
         <v>38</v>
@@ -9597,13 +9657,13 @@
         <v>355</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>769</v>
+        <v>752</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>748</v>
+        <v>731</v>
       </c>
       <c r="F4" s="40" t="s">
         <v>54</v>
@@ -9645,13 +9705,13 @@
         <v>355</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>770</v>
+        <v>753</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>771</v>
+        <v>754</v>
       </c>
       <c r="F5" s="40" t="s">
         <v>54</v>
@@ -10039,18 +10099,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1">
-      <c r="A1" s="92" t="s">
-        <v>890</v>
-      </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
+      <c r="A1" s="94" t="s">
+        <v>872</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
     </row>
     <row r="2" spans="1:11" ht="29" customHeight="1">
       <c r="A2" s="32" t="s">
@@ -10060,25 +10120,25 @@
         <v>6</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>878</v>
+        <v>860</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>880</v>
+        <v>862</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>881</v>
+        <v>863</v>
       </c>
       <c r="F2" s="32" t="s">
         <v>61</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>883</v>
+        <v>865</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>63</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>884</v>
+        <v>866</v>
       </c>
       <c r="J2" s="32" t="s">
         <v>435</v>
@@ -11623,17 +11683,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>452</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="11" t="s">
@@ -11694,25 +11754,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="60" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="11" t="s">
@@ -11801,28 +11861,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="118.75" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>460</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="94"/>
+      <c r="S1" s="94"/>
+      <c r="T1" s="94"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="14" t="s">
@@ -11894,13 +11954,13 @@
         <v>355</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>750</v>
+        <v>733</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>751</v>
+        <v>734</v>
       </c>
       <c r="F3" s="38" t="s">
         <v>395</v>
@@ -11914,7 +11974,7 @@
         <v>396</v>
       </c>
       <c r="K3" s="38" t="s">
-        <v>752</v>
+        <v>735</v>
       </c>
       <c r="L3" s="38"/>
       <c r="M3" s="38"/>
@@ -11927,7 +11987,7 @@
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="38" t="s">
-        <v>753</v>
+        <v>736</v>
       </c>
       <c r="S3" s="38"/>
       <c r="T3" s="38"/>
@@ -11940,13 +12000,13 @@
         <v>355</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>750</v>
+        <v>733</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>754</v>
+        <v>737</v>
       </c>
       <c r="F4" s="38" t="s">
         <v>395</v>
@@ -11955,7 +12015,7 @@
         <v>82</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>755</v>
+        <v>738</v>
       </c>
       <c r="I4" s="38" t="s">
         <v>31</v>
@@ -11973,7 +12033,7 @@
       <c r="P4" s="38"/>
       <c r="Q4" s="38"/>
       <c r="R4" s="38" t="s">
-        <v>756</v>
+        <v>739</v>
       </c>
       <c r="S4" s="38"/>
       <c r="T4" s="38"/>
@@ -11986,13 +12046,13 @@
         <v>355</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>750</v>
+        <v>733</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>754</v>
+        <v>737</v>
       </c>
       <c r="F5" s="38" t="s">
         <v>395</v>
@@ -12001,10 +12061,10 @@
         <v>82</v>
       </c>
       <c r="H5" s="38" t="s">
-        <v>755</v>
+        <v>738</v>
       </c>
       <c r="I5" s="38" t="s">
-        <v>757</v>
+        <v>740</v>
       </c>
       <c r="J5" s="38"/>
       <c r="K5" s="38"/>
@@ -12019,7 +12079,7 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="38" t="s">
-        <v>758</v>
+        <v>741</v>
       </c>
       <c r="S5" s="38"/>
       <c r="T5" s="38"/>
@@ -12032,13 +12092,13 @@
         <v>355</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>759</v>
+        <v>742</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>751</v>
+        <v>734</v>
       </c>
       <c r="F6" s="38" t="s">
         <v>395</v>
@@ -12052,7 +12112,7 @@
         <v>396</v>
       </c>
       <c r="K6" s="38" t="s">
-        <v>752</v>
+        <v>735</v>
       </c>
       <c r="L6" s="38"/>
       <c r="M6" s="38"/>
@@ -12065,7 +12125,7 @@
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="38" t="s">
-        <v>760</v>
+        <v>743</v>
       </c>
       <c r="S6" s="38"/>
       <c r="T6" s="38"/>
@@ -12078,13 +12138,13 @@
         <v>355</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>759</v>
+        <v>742</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>754</v>
+        <v>737</v>
       </c>
       <c r="F7" s="38" t="s">
         <v>395</v>
@@ -12093,10 +12153,10 @@
         <v>82</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>755</v>
+        <v>738</v>
       </c>
       <c r="I7" s="38" t="s">
-        <v>757</v>
+        <v>740</v>
       </c>
       <c r="J7" s="38"/>
       <c r="K7" s="38"/>
@@ -12111,7 +12171,7 @@
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
       <c r="R7" s="38" t="s">
-        <v>761</v>
+        <v>744</v>
       </c>
       <c r="S7" s="38"/>
       <c r="T7" s="38"/>
@@ -12124,13 +12184,13 @@
         <v>355</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>759</v>
+        <v>742</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>754</v>
+        <v>737</v>
       </c>
       <c r="F8" s="38" t="s">
         <v>395</v>
@@ -12139,10 +12199,10 @@
         <v>82</v>
       </c>
       <c r="H8" s="38" t="s">
-        <v>755</v>
+        <v>738</v>
       </c>
       <c r="I8" s="38" t="s">
-        <v>762</v>
+        <v>745</v>
       </c>
       <c r="J8" s="38"/>
       <c r="K8" s="38"/>
@@ -12157,7 +12217,7 @@
       <c r="P8" s="38"/>
       <c r="Q8" s="38"/>
       <c r="R8" s="38" t="s">
-        <v>763</v>
+        <v>746</v>
       </c>
       <c r="S8" s="38"/>
       <c r="T8" s="38"/>
@@ -12170,13 +12230,13 @@
         <v>355</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>759</v>
+        <v>742</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>751</v>
+        <v>734</v>
       </c>
       <c r="F9" s="38" t="s">
         <v>395</v>
@@ -12190,7 +12250,7 @@
         <v>396</v>
       </c>
       <c r="K9" s="38" t="s">
-        <v>764</v>
+        <v>747</v>
       </c>
       <c r="L9" s="38"/>
       <c r="M9" s="38"/>
@@ -12203,7 +12263,7 @@
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
       <c r="R9" s="38" t="s">
-        <v>765</v>
+        <v>748</v>
       </c>
       <c r="S9" s="38"/>
       <c r="T9" s="38"/>
@@ -12216,13 +12276,13 @@
         <v>355</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>764</v>
+        <v>747</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>751</v>
+        <v>734</v>
       </c>
       <c r="F10" s="38" t="s">
         <v>395</v>
@@ -12233,10 +12293,10 @@
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38" t="s">
-        <v>775</v>
+        <v>758</v>
       </c>
       <c r="K10" s="38" t="s">
-        <v>776</v>
+        <v>759</v>
       </c>
       <c r="L10" s="38"/>
       <c r="M10" s="38"/>
@@ -12249,7 +12309,7 @@
       <c r="P10" s="38"/>
       <c r="Q10" s="38"/>
       <c r="R10" s="38" t="s">
-        <v>777</v>
+        <v>760</v>
       </c>
       <c r="S10" s="38"/>
       <c r="T10" s="38"/>
@@ -12262,13 +12322,13 @@
         <v>355</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>764</v>
+        <v>747</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>754</v>
+        <v>737</v>
       </c>
       <c r="F11" s="38" t="s">
         <v>395</v>
@@ -12277,10 +12337,10 @@
         <v>82</v>
       </c>
       <c r="H11" s="38" t="s">
-        <v>778</v>
+        <v>761</v>
       </c>
       <c r="I11" s="38" t="s">
-        <v>752</v>
+        <v>735</v>
       </c>
       <c r="J11" s="38"/>
       <c r="K11" s="38"/>
@@ -12295,7 +12355,7 @@
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
       <c r="R11" s="38" t="s">
-        <v>779</v>
+        <v>762</v>
       </c>
       <c r="S11" s="38"/>
       <c r="T11" s="38"/>
@@ -12308,13 +12368,13 @@
         <v>355</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>764</v>
+        <v>747</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>754</v>
+        <v>737</v>
       </c>
       <c r="F12" s="38" t="s">
         <v>395</v>
@@ -12323,10 +12383,10 @@
         <v>82</v>
       </c>
       <c r="H12" s="38" t="s">
-        <v>778</v>
+        <v>761</v>
       </c>
       <c r="I12" s="38" t="s">
-        <v>759</v>
+        <v>742</v>
       </c>
       <c r="J12" s="38"/>
       <c r="K12" s="38"/>
@@ -12341,7 +12401,7 @@
       <c r="P12" s="38"/>
       <c r="Q12" s="38"/>
       <c r="R12" s="38" t="s">
-        <v>780</v>
+        <v>763</v>
       </c>
       <c r="S12" s="38"/>
       <c r="T12" s="38"/>
@@ -12354,13 +12414,13 @@
         <v>355</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>752</v>
+        <v>735</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>751</v>
+        <v>734</v>
       </c>
       <c r="F13" s="38" t="s">
         <v>395</v>
@@ -12374,7 +12434,7 @@
         <v>396</v>
       </c>
       <c r="K13" s="38" t="s">
-        <v>764</v>
+        <v>747</v>
       </c>
       <c r="L13" s="38"/>
       <c r="M13" s="38"/>
@@ -12387,7 +12447,7 @@
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
       <c r="R13" s="38" t="s">
-        <v>781</v>
+        <v>764</v>
       </c>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
@@ -12400,13 +12460,13 @@
         <v>355</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>752</v>
+        <v>735</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>751</v>
+        <v>734</v>
       </c>
       <c r="F14" s="38" t="s">
         <v>395</v>
@@ -12417,10 +12477,10 @@
       <c r="H14" s="38"/>
       <c r="I14" s="38"/>
       <c r="J14" s="38" t="s">
-        <v>775</v>
+        <v>758</v>
       </c>
       <c r="K14" s="38" t="s">
-        <v>776</v>
+        <v>759</v>
       </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
@@ -12433,7 +12493,7 @@
       <c r="P14" s="38"/>
       <c r="Q14" s="38"/>
       <c r="R14" s="38" t="s">
-        <v>777</v>
+        <v>760</v>
       </c>
       <c r="S14" s="38"/>
       <c r="T14" s="38"/>
@@ -12446,13 +12506,13 @@
         <v>355</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>752</v>
+        <v>735</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>754</v>
+        <v>737</v>
       </c>
       <c r="F15" s="38" t="s">
         <v>395</v>
@@ -12461,10 +12521,10 @@
         <v>82</v>
       </c>
       <c r="H15" s="38" t="s">
-        <v>778</v>
+        <v>761</v>
       </c>
       <c r="I15" s="38" t="s">
-        <v>750</v>
+        <v>733</v>
       </c>
       <c r="J15" s="38"/>
       <c r="K15" s="38"/>
@@ -12479,7 +12539,7 @@
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
       <c r="R15" s="38" t="s">
-        <v>782</v>
+        <v>765</v>
       </c>
       <c r="S15" s="38"/>
       <c r="T15" s="38"/>
@@ -12492,13 +12552,13 @@
         <v>355</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>752</v>
+        <v>735</v>
       </c>
       <c r="E16" s="38" t="s">
-        <v>754</v>
+        <v>737</v>
       </c>
       <c r="F16" s="38" t="s">
         <v>395</v>
@@ -12507,10 +12567,10 @@
         <v>82</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>778</v>
+        <v>761</v>
       </c>
       <c r="I16" s="38" t="s">
-        <v>759</v>
+        <v>742</v>
       </c>
       <c r="J16" s="38"/>
       <c r="K16" s="38"/>
@@ -12525,7 +12585,7 @@
       <c r="P16" s="38"/>
       <c r="Q16" s="38"/>
       <c r="R16" s="38" t="s">
-        <v>780</v>
+        <v>763</v>
       </c>
       <c r="S16" s="38"/>
       <c r="T16" s="38"/>
@@ -12745,15 +12805,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="72.75" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>461</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
     </row>
     <row r="2" spans="1:7" s="47" customFormat="1" ht="28.75" customHeight="1">
       <c r="A2" s="32" t="s">
@@ -12891,26 +12951,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="117" customHeight="1">
-      <c r="A1" s="100" t="s">
-        <v>877</v>
-      </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="93" t="s">
+      <c r="A1" s="102" t="s">
+        <v>859</v>
+      </c>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="95" t="s">
         <v>586</v>
       </c>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="95"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="97"/>
     </row>
     <row r="2" spans="1:18" s="47" customFormat="1" ht="52.25" customHeight="1">
       <c r="A2" s="32" t="s">
@@ -12993,13 +13053,13 @@
         <v>59</v>
       </c>
       <c r="D4" s="63" t="s">
-        <v>772</v>
+        <v>755</v>
       </c>
       <c r="E4" s="63" t="s">
         <v>354</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>808</v>
+        <v>790</v>
       </c>
       <c r="G4" s="63" t="b">
         <v>0</v>
@@ -13043,13 +13103,13 @@
         <v>59</v>
       </c>
       <c r="D5" s="63" t="s">
-        <v>773</v>
+        <v>756</v>
       </c>
       <c r="E5" s="63" t="s">
         <v>108</v>
       </c>
       <c r="F5" s="63" t="s">
-        <v>809</v>
+        <v>791</v>
       </c>
       <c r="G5" s="63" t="b">
         <v>0</v>
@@ -13087,13 +13147,13 @@
         <v>59</v>
       </c>
       <c r="D6" s="63" t="s">
-        <v>774</v>
+        <v>757</v>
       </c>
       <c r="E6" s="63" t="s">
         <v>354</v>
       </c>
       <c r="F6" s="63" t="s">
-        <v>809</v>
+        <v>791</v>
       </c>
       <c r="G6" s="63" t="b">
         <v>0</v>
@@ -13131,13 +13191,13 @@
         <v>59</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>770</v>
+        <v>753</v>
       </c>
       <c r="E7" s="63" t="s">
         <v>108</v>
       </c>
       <c r="F7" s="63" t="s">
-        <v>810</v>
+        <v>792</v>
       </c>
       <c r="G7" s="63" t="b">
         <v>0</v>
@@ -13196,18 +13256,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="114.75" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>587</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="95"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="97"/>
     </row>
     <row r="2" spans="1:10" s="47" customFormat="1" ht="28.75" customHeight="1">
       <c r="A2" s="11" t="s">
@@ -13263,7 +13323,7 @@
         <v>328</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>783</v>
+        <v>766</v>
       </c>
       <c r="D4" s="63">
         <v>150</v>
@@ -13272,7 +13332,7 @@
         <v>59</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>774</v>
+        <v>757</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>114</v>
@@ -13295,7 +13355,7 @@
         <v>336</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>784</v>
+        <v>767</v>
       </c>
       <c r="D5" s="63">
         <v>150</v>
@@ -13304,7 +13364,7 @@
         <v>59</v>
       </c>
       <c r="F5" s="63" t="s">
-        <v>770</v>
+        <v>753</v>
       </c>
       <c r="G5" s="63" t="s">
         <v>114</v>
@@ -13353,27 +13413,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="110.5" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="105" t="s">
         <v>468</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="106" t="s">
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="108" t="s">
         <v>462</v>
       </c>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106"/>
-      <c r="Q1" s="106"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="51.75" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -13473,7 +13533,7 @@
         <v>129</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>813</v>
+        <v>795</v>
       </c>
       <c r="J4" s="30"/>
       <c r="K4" s="30"/>
@@ -13498,7 +13558,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
       <c r="I5" s="30" t="s">
-        <v>813</v>
+        <v>795</v>
       </c>
       <c r="J5" s="30" t="s">
         <v>130</v>
@@ -13522,7 +13582,7 @@
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30" t="s">
-        <v>813</v>
+        <v>795</v>
       </c>
       <c r="J6" s="30" t="s">
         <v>132</v>
@@ -13559,7 +13619,7 @@
         <v>134</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>814</v>
+        <v>796</v>
       </c>
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
@@ -13592,7 +13652,7 @@
         <v>136</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>815</v>
+        <v>797</v>
       </c>
       <c r="J8" s="30" t="s">
         <v>137</v>
@@ -13631,7 +13691,7 @@
         <v>136</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>815</v>
+        <v>797</v>
       </c>
       <c r="J9" s="30" t="s">
         <v>139</v>
@@ -13668,7 +13728,7 @@
         <v>141</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>816</v>
+        <v>798</v>
       </c>
       <c r="J10" s="30"/>
       <c r="K10" s="30"/>
@@ -13712,24 +13772,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="122.5" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>454</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
     </row>
     <row r="2" spans="1:16" ht="43.25" customHeight="1">
       <c r="A2" s="21" t="s">
@@ -13940,13 +14000,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="47" customFormat="1" ht="108" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>447</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="32" t="s">
@@ -14187,29 +14247,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="87.75" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>474</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="94"/>
-      <c r="U1" s="95"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="97"/>
     </row>
     <row r="2" spans="1:21" ht="58.25" customHeight="1">
       <c r="A2" s="41" t="s">
@@ -14489,29 +14549,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="115.75" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>445</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="96" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="98" t="s">
         <v>470</v>
       </c>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="107"/>
-      <c r="S1" s="108"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="109"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="109"/>
+      <c r="S1" s="110"/>
     </row>
     <row r="2" spans="1:19" ht="58.75" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -15176,14 +15236,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="47" customFormat="1" ht="44.5" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="111" t="s">
         <v>446</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="111"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="113"/>
     </row>
     <row r="2" spans="1:6" ht="14.5" customHeight="1">
       <c r="A2" s="21" t="s">
@@ -15320,24 +15380,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="88.25" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>473</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
     </row>
     <row r="2" spans="1:16" ht="46.25" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -15553,17 +15613,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="114" customHeight="1">
-      <c r="A1" s="112" t="s">
-        <v>817</v>
-      </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
+      <c r="A1" s="114" t="s">
+        <v>799</v>
+      </c>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="8" t="s">
@@ -15576,19 +15636,19 @@
         <v>323</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>818</v>
+        <v>800</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>819</v>
+        <v>801</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>820</v>
+        <v>802</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>821</v>
+        <v>803</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>822</v>
+        <v>804</v>
       </c>
       <c r="I2" s="32" t="s">
         <v>435</v>
@@ -15615,13 +15675,13 @@
         <v>355</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>823</v>
+        <v>805</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>824</v>
+        <v>806</v>
       </c>
       <c r="E4" s="72" t="s">
-        <v>825</v>
+        <v>807</v>
       </c>
       <c r="F4" s="40">
         <v>1</v>
@@ -15630,7 +15690,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>826</v>
+        <v>808</v>
       </c>
       <c r="I4" s="60" t="s">
         <v>455</v>
@@ -15645,13 +15705,13 @@
         <v>355</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>827</v>
+        <v>809</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>828</v>
+        <v>810</v>
       </c>
       <c r="E5" s="72" t="s">
-        <v>825</v>
+        <v>807</v>
       </c>
       <c r="F5" s="40">
         <v>1</v>
@@ -15660,7 +15720,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>829</v>
+        <v>811</v>
       </c>
       <c r="I5" s="49"/>
       <c r="J5" s="51"/>
@@ -15708,32 +15768,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="73" customFormat="1" ht="135.75" customHeight="1">
-      <c r="A1" s="93" t="s">
-        <v>830</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="94"/>
-      <c r="U1" s="94"/>
-      <c r="V1" s="94"/>
-      <c r="W1" s="94"/>
-      <c r="X1" s="95"/>
+      <c r="A1" s="95" t="s">
+        <v>812</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="97"/>
     </row>
     <row r="2" spans="1:24" s="76" customFormat="1" ht="43.5">
       <c r="A2" s="74" t="s">
@@ -15749,49 +15809,49 @@
         <v>88</v>
       </c>
       <c r="E2" s="75" t="s">
-        <v>831</v>
+        <v>813</v>
       </c>
       <c r="F2" s="74" t="s">
         <v>89</v>
       </c>
       <c r="G2" s="74" t="s">
-        <v>832</v>
+        <v>814</v>
       </c>
       <c r="H2" s="74" t="s">
-        <v>833</v>
+        <v>815</v>
       </c>
       <c r="I2" s="74" t="s">
-        <v>834</v>
+        <v>816</v>
       </c>
       <c r="J2" s="74" t="s">
-        <v>835</v>
+        <v>817</v>
       </c>
       <c r="K2" s="75" t="s">
         <v>411</v>
       </c>
       <c r="L2" s="74" t="s">
-        <v>836</v>
+        <v>818</v>
       </c>
       <c r="M2" s="74" t="s">
-        <v>837</v>
+        <v>819</v>
       </c>
       <c r="N2" s="74" t="s">
-        <v>838</v>
+        <v>820</v>
       </c>
       <c r="O2" s="74" t="s">
-        <v>839</v>
+        <v>821</v>
       </c>
       <c r="P2" s="74" t="s">
-        <v>840</v>
+        <v>822</v>
       </c>
       <c r="Q2" s="74" t="s">
-        <v>841</v>
+        <v>823</v>
       </c>
       <c r="R2" s="74" t="s">
-        <v>842</v>
+        <v>824</v>
       </c>
       <c r="S2" s="74" t="s">
-        <v>843</v>
+        <v>825</v>
       </c>
       <c r="T2" s="74" t="s">
         <v>326</v>
@@ -15800,10 +15860,10 @@
         <v>327</v>
       </c>
       <c r="V2" s="74" t="s">
-        <v>844</v>
+        <v>826</v>
       </c>
       <c r="W2" s="74" t="s">
-        <v>845</v>
+        <v>827</v>
       </c>
       <c r="X2" s="74" t="s">
         <v>435</v>
@@ -15845,13 +15905,13 @@
         <v>355</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>846</v>
+        <v>828</v>
       </c>
       <c r="D4" s="53" t="s">
         <v>59</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>847</v>
+        <v>829</v>
       </c>
       <c r="F4" s="53" t="s">
         <v>340</v>
@@ -15866,25 +15926,25 @@
         <v>256</v>
       </c>
       <c r="J4" s="53" t="s">
-        <v>848</v>
+        <v>830</v>
       </c>
       <c r="K4" s="53" t="s">
         <v>331</v>
       </c>
       <c r="L4" s="53" t="s">
-        <v>849</v>
+        <v>831</v>
       </c>
       <c r="M4" s="53" t="s">
-        <v>850</v>
+        <v>832</v>
       </c>
       <c r="N4" s="77" t="s">
         <v>412</v>
       </c>
       <c r="O4" s="53" t="s">
-        <v>851</v>
+        <v>833</v>
       </c>
       <c r="P4" s="53" t="s">
-        <v>852</v>
+        <v>834</v>
       </c>
       <c r="Q4" s="53" t="s">
         <v>333</v>
@@ -15905,10 +15965,10 @@
         <v>15</v>
       </c>
       <c r="W4" s="40" t="s">
-        <v>853</v>
+        <v>835</v>
       </c>
       <c r="X4" s="40" t="s">
-        <v>854</v>
+        <v>836</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -15919,13 +15979,13 @@
         <v>355</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>855</v>
+        <v>837</v>
       </c>
       <c r="D5" s="53" t="s">
         <v>103</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>856</v>
+        <v>838</v>
       </c>
       <c r="F5" s="53" t="s">
         <v>339</v>
@@ -15940,25 +16000,25 @@
         <v>256</v>
       </c>
       <c r="J5" s="53" t="s">
-        <v>848</v>
+        <v>830</v>
       </c>
       <c r="K5" s="53" t="s">
         <v>413</v>
       </c>
       <c r="L5" s="53" t="s">
-        <v>857</v>
+        <v>839</v>
       </c>
       <c r="M5" s="53" t="s">
-        <v>858</v>
+        <v>840</v>
       </c>
       <c r="N5" s="77" t="s">
         <v>414</v>
       </c>
       <c r="O5" s="53" t="s">
-        <v>859</v>
+        <v>841</v>
       </c>
       <c r="P5" s="53" t="s">
-        <v>852</v>
+        <v>834</v>
       </c>
       <c r="Q5" s="53" t="s">
         <v>333</v>
@@ -15979,10 +16039,10 @@
         <v>15</v>
       </c>
       <c r="W5" s="40" t="s">
-        <v>860</v>
+        <v>842</v>
       </c>
       <c r="X5" s="40" t="s">
-        <v>861</v>
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -16058,32 +16118,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="73" customFormat="1" ht="133.25" customHeight="1">
-      <c r="A1" s="93" t="s">
-        <v>862</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="94"/>
-      <c r="U1" s="94"/>
-      <c r="V1" s="94"/>
-      <c r="W1" s="94"/>
-      <c r="X1" s="95"/>
+      <c r="A1" s="95" t="s">
+        <v>844</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="97"/>
     </row>
     <row r="2" spans="1:24" s="76" customFormat="1" ht="29">
       <c r="A2" s="74" t="s">
@@ -16099,49 +16159,49 @@
         <v>88</v>
       </c>
       <c r="E2" s="75" t="s">
-        <v>831</v>
+        <v>813</v>
       </c>
       <c r="F2" s="74" t="s">
         <v>89</v>
       </c>
       <c r="G2" s="74" t="s">
-        <v>863</v>
+        <v>845</v>
       </c>
       <c r="H2" s="74" t="s">
-        <v>833</v>
+        <v>815</v>
       </c>
       <c r="I2" s="74" t="s">
-        <v>834</v>
+        <v>816</v>
       </c>
       <c r="J2" s="74" t="s">
-        <v>835</v>
+        <v>817</v>
       </c>
       <c r="K2" s="79" t="s">
         <v>411</v>
       </c>
       <c r="L2" s="74" t="s">
-        <v>836</v>
+        <v>818</v>
       </c>
       <c r="M2" s="74" t="s">
-        <v>837</v>
+        <v>819</v>
       </c>
       <c r="N2" s="74" t="s">
-        <v>838</v>
+        <v>820</v>
       </c>
       <c r="O2" s="74" t="s">
-        <v>839</v>
+        <v>821</v>
       </c>
       <c r="P2" s="74" t="s">
-        <v>840</v>
+        <v>822</v>
       </c>
       <c r="Q2" s="74" t="s">
-        <v>841</v>
+        <v>823</v>
       </c>
       <c r="R2" s="74" t="s">
-        <v>842</v>
+        <v>824</v>
       </c>
       <c r="S2" s="74" t="s">
-        <v>843</v>
+        <v>825</v>
       </c>
       <c r="T2" s="74" t="s">
         <v>326</v>
@@ -16150,10 +16210,10 @@
         <v>327</v>
       </c>
       <c r="V2" s="74" t="s">
-        <v>844</v>
+        <v>826</v>
       </c>
       <c r="W2" s="74" t="s">
-        <v>845</v>
+        <v>827</v>
       </c>
       <c r="X2" s="80" t="s">
         <v>435</v>
@@ -16195,13 +16255,13 @@
         <v>355</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>846</v>
+        <v>828</v>
       </c>
       <c r="D4" s="53" t="s">
         <v>59</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>864</v>
+        <v>846</v>
       </c>
       <c r="F4" s="53" t="s">
         <v>342</v>
@@ -16216,25 +16276,25 @@
         <v>256</v>
       </c>
       <c r="J4" s="53" t="s">
-        <v>848</v>
+        <v>830</v>
       </c>
       <c r="K4" s="53" t="s">
         <v>331</v>
       </c>
       <c r="L4" s="53" t="s">
-        <v>865</v>
+        <v>847</v>
       </c>
       <c r="M4" s="53" t="s">
-        <v>866</v>
+        <v>848</v>
       </c>
       <c r="N4" s="53" t="s">
         <v>332</v>
       </c>
       <c r="O4" s="53" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="P4" s="53" t="s">
-        <v>852</v>
+        <v>834</v>
       </c>
       <c r="Q4" s="53" t="s">
         <v>333</v>
@@ -16255,7 +16315,7 @@
         <v>15</v>
       </c>
       <c r="W4" s="40" t="s">
-        <v>868</v>
+        <v>850</v>
       </c>
       <c r="X4" s="38" t="s">
         <v>455</v>
@@ -16269,13 +16329,13 @@
         <v>355</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>855</v>
+        <v>837</v>
       </c>
       <c r="D5" s="53" t="s">
         <v>59</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="F5" s="53" t="s">
         <v>344</v>
@@ -16290,25 +16350,25 @@
         <v>256</v>
       </c>
       <c r="J5" s="53" t="s">
-        <v>848</v>
+        <v>830</v>
       </c>
       <c r="K5" s="53" t="s">
         <v>413</v>
       </c>
       <c r="L5" s="53" t="s">
-        <v>870</v>
+        <v>852</v>
       </c>
       <c r="M5" s="53" t="s">
-        <v>871</v>
+        <v>853</v>
       </c>
       <c r="N5" s="53" t="s">
         <v>416</v>
       </c>
       <c r="O5" s="53" t="s">
-        <v>872</v>
+        <v>854</v>
       </c>
       <c r="P5" s="53" t="s">
-        <v>852</v>
+        <v>834</v>
       </c>
       <c r="Q5" s="53" t="s">
         <v>333</v>
@@ -16329,7 +16389,7 @@
         <v>15</v>
       </c>
       <c r="W5" s="81" t="s">
-        <v>853</v>
+        <v>835</v>
       </c>
       <c r="X5" s="40"/>
     </row>
@@ -16407,32 +16467,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="73" customFormat="1" ht="195" customHeight="1">
-      <c r="A1" s="93" t="s">
-        <v>873</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="94"/>
-      <c r="U1" s="94"/>
-      <c r="V1" s="94"/>
-      <c r="W1" s="94"/>
-      <c r="X1" s="95"/>
+      <c r="A1" s="95" t="s">
+        <v>855</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="97"/>
     </row>
     <row r="2" spans="1:24" s="76" customFormat="1" ht="29">
       <c r="A2" s="74" t="s">
@@ -16448,49 +16508,49 @@
         <v>88</v>
       </c>
       <c r="E2" s="74" t="s">
-        <v>874</v>
+        <v>856</v>
       </c>
       <c r="F2" s="75" t="s">
-        <v>831</v>
+        <v>813</v>
       </c>
       <c r="G2" s="74" t="s">
         <v>89</v>
       </c>
       <c r="H2" s="74" t="s">
-        <v>863</v>
+        <v>845</v>
       </c>
       <c r="I2" s="74" t="s">
-        <v>834</v>
+        <v>816</v>
       </c>
       <c r="J2" s="74" t="s">
-        <v>835</v>
+        <v>817</v>
       </c>
       <c r="K2" s="75" t="s">
         <v>411</v>
       </c>
       <c r="L2" s="74" t="s">
-        <v>836</v>
+        <v>818</v>
       </c>
       <c r="M2" s="74" t="s">
-        <v>818</v>
+        <v>800</v>
       </c>
       <c r="N2" s="74" t="s">
-        <v>838</v>
+        <v>820</v>
       </c>
       <c r="O2" s="74" t="s">
-        <v>839</v>
+        <v>821</v>
       </c>
       <c r="P2" s="74" t="s">
-        <v>840</v>
+        <v>822</v>
       </c>
       <c r="Q2" s="74" t="s">
-        <v>841</v>
+        <v>823</v>
       </c>
       <c r="R2" s="74" t="s">
-        <v>842</v>
+        <v>824</v>
       </c>
       <c r="S2" s="74" t="s">
-        <v>843</v>
+        <v>825</v>
       </c>
       <c r="T2" s="74" t="s">
         <v>326</v>
@@ -16499,10 +16559,10 @@
         <v>327</v>
       </c>
       <c r="V2" s="74" t="s">
-        <v>844</v>
+        <v>826</v>
       </c>
       <c r="W2" s="74" t="s">
-        <v>845</v>
+        <v>827</v>
       </c>
       <c r="X2" s="21" t="s">
         <v>435</v>
@@ -16543,16 +16603,16 @@
         <v>355</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>846</v>
+        <v>828</v>
       </c>
       <c r="D4" s="53" t="s">
         <v>59</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>855</v>
+        <v>837</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>875</v>
+        <v>857</v>
       </c>
       <c r="G4" s="53" t="s">
         <v>346</v>
@@ -16564,25 +16624,25 @@
         <v>256</v>
       </c>
       <c r="J4" s="53" t="s">
-        <v>848</v>
+        <v>830</v>
       </c>
       <c r="K4" s="53" t="s">
         <v>331</v>
       </c>
       <c r="L4" s="53" t="s">
-        <v>876</v>
+        <v>858</v>
       </c>
       <c r="M4" s="53" t="s">
-        <v>850</v>
+        <v>832</v>
       </c>
       <c r="N4" s="53" t="s">
         <v>332</v>
       </c>
       <c r="O4" s="53" t="s">
-        <v>851</v>
+        <v>833</v>
       </c>
       <c r="P4" s="53" t="s">
-        <v>852</v>
+        <v>834</v>
       </c>
       <c r="Q4" s="53" t="s">
         <v>333</v>
@@ -16603,7 +16663,7 @@
         <v>10</v>
       </c>
       <c r="W4" s="81" t="s">
-        <v>853</v>
+        <v>835</v>
       </c>
       <c r="X4" s="38" t="s">
         <v>455</v>
@@ -17737,10 +17797,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -17753,13 +17813,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="47" customFormat="1" ht="105.75" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>448</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
@@ -17861,16 +17921,29 @@
         <v>5</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>786</v>
+        <v>769</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>785</v>
+        <v>768</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="60" t="s">
+    <row r="10" spans="1:5" s="51" customFormat="1" ht="28" customHeight="1">
+      <c r="A10" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>879</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>880</v>
+      </c>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="92" t="s">
         <v>4</v>
       </c>
     </row>
@@ -17885,10 +17958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:H154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -17903,16 +17976,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="47" customFormat="1" ht="102.75" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>449</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
     </row>
     <row r="2" spans="1:8" s="47" customFormat="1">
       <c r="A2" s="7" t="s">
@@ -17940,53 +18013,53 @@
         <v>435</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="3" spans="1:8" s="39" customFormat="1" ht="69.5" customHeight="1">
       <c r="A3" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>787</v>
+        <v>770</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>406</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>792</v>
+        <v>775</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>793</v>
+        <v>776</v>
       </c>
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
       <c r="H3" s="38"/>
     </row>
-    <row r="4" spans="1:8" s="39" customFormat="1" ht="102.5" customHeight="1">
-      <c r="A4" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>607</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>608</v>
-      </c>
+    <row r="4" spans="1:8" s="39" customFormat="1" ht="69.5" customHeight="1">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="38" t="s">
-        <v>609</v>
+        <v>876</v>
       </c>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
       <c r="H4" s="38"/>
     </row>
-    <row r="5" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
+    <row r="5" spans="1:8" s="39" customFormat="1" ht="102.5" customHeight="1">
+      <c r="A5" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>607</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>608</v>
+      </c>
       <c r="E5" s="38" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
@@ -17998,7 +18071,7 @@
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
@@ -18010,7 +18083,7 @@
       <c r="C7" s="38"/>
       <c r="D7" s="38"/>
       <c r="E7" s="38" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
@@ -18022,7 +18095,7 @@
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
       <c r="E8" s="38" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
@@ -18034,7 +18107,7 @@
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
       <c r="E9" s="38" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
@@ -18046,7 +18119,7 @@
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
@@ -18058,7 +18131,7 @@
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
       <c r="E11" s="38" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
@@ -18070,7 +18143,7 @@
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
       <c r="E12" s="38" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F12" s="38"/>
       <c r="G12" s="38"/>
@@ -18082,7 +18155,7 @@
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
       <c r="E13" s="38" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
@@ -18094,7 +18167,7 @@
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
       <c r="E14" s="38" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
@@ -18106,7 +18179,7 @@
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
       <c r="E15" s="38" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F15" s="38"/>
       <c r="G15" s="38"/>
@@ -18118,7 +18191,7 @@
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
       <c r="E16" s="38" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F16" s="38"/>
       <c r="G16" s="38"/>
@@ -18130,7 +18203,7 @@
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
       <c r="E17" s="38" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F17" s="38"/>
       <c r="G17" s="38"/>
@@ -18142,7 +18215,7 @@
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
       <c r="E18" s="38" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F18" s="38"/>
       <c r="G18" s="38"/>
@@ -18154,7 +18227,7 @@
       <c r="C19" s="38"/>
       <c r="D19" s="38"/>
       <c r="E19" s="38" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F19" s="38"/>
       <c r="G19" s="38"/>
@@ -18166,31 +18239,31 @@
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
       <c r="E20" s="38" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F20" s="38"/>
       <c r="G20" s="38"/>
       <c r="H20" s="38"/>
     </row>
-    <row r="21" spans="1:8" s="39" customFormat="1" ht="29">
+    <row r="21" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="38" t="s">
-        <v>789</v>
+        <v>625</v>
       </c>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
       <c r="H21" s="38"/>
     </row>
-    <row r="22" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="22" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A22" s="38"/>
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
       <c r="E22" s="38" t="s">
-        <v>788</v>
+        <v>772</v>
       </c>
       <c r="F22" s="38"/>
       <c r="G22" s="38"/>
@@ -18202,7 +18275,7 @@
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
       <c r="E23" s="38" t="s">
-        <v>626</v>
+        <v>771</v>
       </c>
       <c r="F23" s="38"/>
       <c r="G23" s="38"/>
@@ -18214,7 +18287,7 @@
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
       <c r="E24" s="38" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F24" s="38"/>
       <c r="G24" s="38"/>
@@ -18226,7 +18299,7 @@
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
       <c r="E25" s="38" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
@@ -18238,19 +18311,19 @@
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
       <c r="E26" s="38" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
       <c r="H26" s="38"/>
     </row>
-    <row r="27" spans="1:8" s="39" customFormat="1">
+    <row r="27" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A27" s="38"/>
       <c r="B27" s="38"/>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>
       <c r="E27" s="38" t="s">
-        <v>630</v>
+        <v>887</v>
       </c>
       <c r="F27" s="38"/>
       <c r="G27" s="38"/>
@@ -18262,63 +18335,55 @@
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
       <c r="E28" s="38" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
       <c r="H28" s="38"/>
     </row>
-    <row r="29" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="29" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A29" s="38"/>
       <c r="B29" s="38"/>
       <c r="C29" s="38"/>
       <c r="D29" s="38"/>
       <c r="E29" s="38" t="s">
-        <v>632</v>
+        <v>888</v>
       </c>
       <c r="F29" s="38"/>
       <c r="G29" s="38"/>
       <c r="H29" s="38"/>
     </row>
-    <row r="30" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="30" spans="1:8" s="39" customFormat="1">
       <c r="A30" s="38"/>
       <c r="B30" s="38"/>
       <c r="C30" s="38"/>
       <c r="D30" s="38"/>
       <c r="E30" s="38" t="s">
-        <v>633</v>
+        <v>889</v>
       </c>
       <c r="F30" s="38"/>
       <c r="G30" s="38"/>
       <c r="H30" s="38"/>
     </row>
-    <row r="31" spans="1:8" s="39" customFormat="1" ht="29">
+    <row r="31" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A31" s="38"/>
       <c r="B31" s="38"/>
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
       <c r="E31" s="38" t="s">
-        <v>790</v>
+        <v>630</v>
       </c>
       <c r="F31" s="38"/>
       <c r="G31" s="38"/>
       <c r="H31" s="38"/>
     </row>
-    <row r="32" spans="1:8" s="39" customFormat="1" ht="43.5" customHeight="1">
-      <c r="A32" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>634</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>635</v>
-      </c>
+    <row r="32" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A32" s="38"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="38" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="F32" s="38"/>
       <c r="G32" s="38"/>
@@ -18330,55 +18395,63 @@
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
       <c r="E33" s="38" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="F33" s="38"/>
       <c r="G33" s="38"/>
       <c r="H33" s="38"/>
     </row>
-    <row r="34" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="34" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A34" s="38"/>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
       <c r="D34" s="38"/>
       <c r="E34" s="38" t="s">
-        <v>638</v>
+        <v>773</v>
       </c>
       <c r="F34" s="38"/>
       <c r="G34" s="38"/>
       <c r="H34" s="38"/>
     </row>
-    <row r="35" spans="1:8" s="39" customFormat="1" ht="43.5" customHeight="1">
+    <row r="35" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A35" s="38"/>
       <c r="B35" s="38"/>
       <c r="C35" s="38"/>
       <c r="D35" s="38"/>
       <c r="E35" s="38" t="s">
-        <v>639</v>
+        <v>891</v>
       </c>
       <c r="F35" s="38"/>
       <c r="G35" s="38"/>
       <c r="H35" s="38"/>
     </row>
-    <row r="36" spans="1:8" s="39" customFormat="1" ht="43.5" customHeight="1">
+    <row r="36" spans="1:8" s="39" customFormat="1">
       <c r="A36" s="38"/>
       <c r="B36" s="38"/>
       <c r="C36" s="38"/>
       <c r="D36" s="38"/>
       <c r="E36" s="38" t="s">
-        <v>640</v>
+        <v>890</v>
       </c>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
       <c r="H36" s="38"/>
     </row>
-    <row r="37" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
-      <c r="A37" s="38"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
+    <row r="37" spans="1:8" s="39" customFormat="1" ht="43.5" customHeight="1">
+      <c r="A37" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>633</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>634</v>
+      </c>
       <c r="E37" s="38" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
@@ -18390,7 +18463,7 @@
       <c r="C38" s="38"/>
       <c r="D38" s="38"/>
       <c r="E38" s="38" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
@@ -18402,31 +18475,31 @@
       <c r="C39" s="38"/>
       <c r="D39" s="38"/>
       <c r="E39" s="38" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
       <c r="H39" s="38"/>
     </row>
-    <row r="40" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="40" spans="1:8" s="39" customFormat="1" ht="43.5" customHeight="1">
       <c r="A40" s="38"/>
       <c r="B40" s="38"/>
       <c r="C40" s="38"/>
       <c r="D40" s="38"/>
       <c r="E40" s="38" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="F40" s="38"/>
       <c r="G40" s="38"/>
       <c r="H40" s="38"/>
     </row>
-    <row r="41" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="41" spans="1:8" s="39" customFormat="1" ht="43.5" customHeight="1">
       <c r="A41" s="38"/>
       <c r="B41" s="38"/>
       <c r="C41" s="38"/>
       <c r="D41" s="38"/>
       <c r="E41" s="38" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="F41" s="38"/>
       <c r="G41" s="38"/>
@@ -18438,39 +18511,31 @@
       <c r="C42" s="38"/>
       <c r="D42" s="38"/>
       <c r="E42" s="38" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="F42" s="38"/>
       <c r="G42" s="38"/>
       <c r="H42" s="38"/>
     </row>
-    <row r="43" spans="1:8" s="39" customFormat="1">
+    <row r="43" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A43" s="38"/>
       <c r="B43" s="38"/>
       <c r="C43" s="38"/>
       <c r="D43" s="38"/>
       <c r="E43" s="38" t="s">
-        <v>791</v>
+        <v>641</v>
       </c>
       <c r="F43" s="38"/>
       <c r="G43" s="38"/>
       <c r="H43" s="38"/>
     </row>
     <row r="44" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
-      <c r="A44" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="38" t="s">
-        <v>647</v>
-      </c>
-      <c r="C44" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="D44" s="38" t="s">
-        <v>648</v>
-      </c>
+      <c r="A44" s="38"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
       <c r="E44" s="38" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="F44" s="38"/>
       <c r="G44" s="38"/>
@@ -18482,139 +18547,155 @@
       <c r="C45" s="38"/>
       <c r="D45" s="38"/>
       <c r="E45" s="38" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="F45" s="38"/>
       <c r="G45" s="38"/>
       <c r="H45" s="38"/>
     </row>
-    <row r="46" spans="1:8" s="39" customFormat="1">
+    <row r="46" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A46" s="38"/>
       <c r="B46" s="38"/>
       <c r="C46" s="38"/>
       <c r="D46" s="38"/>
       <c r="E46" s="38" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="F46" s="38"/>
       <c r="G46" s="38"/>
       <c r="H46" s="38"/>
     </row>
-    <row r="47" spans="1:8" s="39" customFormat="1">
+    <row r="47" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A47" s="38"/>
       <c r="B47" s="38"/>
       <c r="C47" s="38"/>
       <c r="D47" s="38"/>
       <c r="E47" s="38" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="F47" s="38"/>
       <c r="G47" s="38"/>
       <c r="H47" s="38"/>
     </row>
-    <row r="48" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="48" spans="1:8" s="39" customFormat="1">
       <c r="A48" s="38"/>
       <c r="B48" s="38"/>
       <c r="C48" s="38"/>
       <c r="D48" s="38"/>
       <c r="E48" s="38" t="s">
-        <v>653</v>
+        <v>774</v>
       </c>
       <c r="F48" s="38"/>
       <c r="G48" s="38"/>
       <c r="H48" s="38"/>
     </row>
-    <row r="49" spans="1:8" s="39" customFormat="1" ht="29">
+    <row r="49" spans="1:8" s="39" customFormat="1">
       <c r="A49" s="38"/>
       <c r="B49" s="38"/>
       <c r="C49" s="38"/>
       <c r="D49" s="38"/>
       <c r="E49" s="38" t="s">
-        <v>654</v>
+        <v>877</v>
       </c>
       <c r="F49" s="38"/>
       <c r="G49" s="38"/>
       <c r="H49" s="38"/>
     </row>
-    <row r="50" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="50" spans="1:8" s="39" customFormat="1">
       <c r="A50" s="38"/>
       <c r="B50" s="38"/>
       <c r="C50" s="38"/>
       <c r="D50" s="38"/>
       <c r="E50" s="38" t="s">
-        <v>655</v>
+        <v>878</v>
       </c>
       <c r="F50" s="38"/>
       <c r="G50" s="38"/>
       <c r="H50" s="38"/>
     </row>
     <row r="51" spans="1:8" s="39" customFormat="1" ht="29">
-      <c r="A51" s="38"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
+      <c r="A51" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="38" t="s">
+        <v>881</v>
+      </c>
+      <c r="C51" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="D51" s="38" t="s">
+        <v>882</v>
+      </c>
       <c r="E51" s="38" t="s">
-        <v>656</v>
+        <v>883</v>
       </c>
       <c r="F51" s="38"/>
       <c r="G51" s="38"/>
       <c r="H51" s="38"/>
     </row>
-    <row r="52" spans="1:8" s="39" customFormat="1" ht="29">
+    <row r="52" spans="1:8" s="39" customFormat="1">
       <c r="A52" s="38"/>
       <c r="B52" s="38"/>
       <c r="C52" s="38"/>
       <c r="D52" s="38"/>
       <c r="E52" s="38" t="s">
-        <v>657</v>
+        <v>884</v>
       </c>
       <c r="F52" s="38"/>
       <c r="G52" s="38"/>
       <c r="H52" s="38"/>
     </row>
-    <row r="53" spans="1:8" s="39" customFormat="1">
+    <row r="53" spans="1:8" s="39" customFormat="1" ht="203">
       <c r="A53" s="38"/>
       <c r="B53" s="38"/>
       <c r="C53" s="38"/>
       <c r="D53" s="38"/>
       <c r="E53" s="38" t="s">
-        <v>658</v>
+        <v>885</v>
       </c>
       <c r="F53" s="38"/>
       <c r="G53" s="38"/>
       <c r="H53" s="38"/>
     </row>
-    <row r="54" spans="1:8" s="39" customFormat="1" ht="29">
+    <row r="54" spans="1:8" s="39" customFormat="1">
       <c r="A54" s="38"/>
       <c r="B54" s="38"/>
       <c r="C54" s="38"/>
       <c r="D54" s="38"/>
       <c r="E54" s="38" t="s">
-        <v>659</v>
+        <v>886</v>
       </c>
       <c r="F54" s="38"/>
       <c r="G54" s="38"/>
       <c r="H54" s="38"/>
     </row>
-    <row r="55" spans="1:8" s="39" customFormat="1">
-      <c r="A55" s="38"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
+    <row r="55" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A55" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="38" t="s">
+        <v>646</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="D55" s="38" t="s">
+        <v>647</v>
+      </c>
       <c r="E55" s="38" t="s">
-        <v>660</v>
+        <v>648</v>
       </c>
       <c r="F55" s="38"/>
       <c r="G55" s="38"/>
       <c r="H55" s="38"/>
     </row>
-    <row r="56" spans="1:8" s="39" customFormat="1">
+    <row r="56" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A56" s="38"/>
       <c r="B56" s="38"/>
       <c r="C56" s="38"/>
       <c r="D56" s="38"/>
       <c r="E56" s="38" t="s">
-        <v>661</v>
+        <v>649</v>
       </c>
       <c r="F56" s="38"/>
       <c r="G56" s="38"/>
@@ -18626,19 +18707,19 @@
       <c r="C57" s="38"/>
       <c r="D57" s="38"/>
       <c r="E57" s="38" t="s">
-        <v>662</v>
+        <v>650</v>
       </c>
       <c r="F57" s="38"/>
       <c r="G57" s="38"/>
       <c r="H57" s="38"/>
     </row>
-    <row r="58" spans="1:8" s="39" customFormat="1" ht="29">
+    <row r="58" spans="1:8" s="39" customFormat="1">
       <c r="A58" s="38"/>
       <c r="B58" s="38"/>
       <c r="C58" s="38"/>
       <c r="D58" s="38"/>
       <c r="E58" s="38" t="s">
-        <v>663</v>
+        <v>651</v>
       </c>
       <c r="F58" s="38"/>
       <c r="G58" s="38"/>
@@ -18650,135 +18731,127 @@
       <c r="C59" s="38"/>
       <c r="D59" s="38"/>
       <c r="E59" s="38" t="s">
-        <v>664</v>
+        <v>652</v>
       </c>
       <c r="F59" s="38"/>
       <c r="G59" s="38"/>
       <c r="H59" s="38"/>
     </row>
-    <row r="60" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="60" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A60" s="38"/>
       <c r="B60" s="38"/>
       <c r="C60" s="38"/>
       <c r="D60" s="38"/>
       <c r="E60" s="38" t="s">
-        <v>665</v>
+        <v>653</v>
       </c>
       <c r="F60" s="38"/>
       <c r="G60" s="38"/>
       <c r="H60" s="38"/>
     </row>
-    <row r="61" spans="1:8" s="39" customFormat="1" ht="87" customHeight="1">
-      <c r="A61" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61" s="38" t="s">
-        <v>666</v>
-      </c>
-      <c r="C61" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="D61" s="38" t="s">
-        <v>667</v>
-      </c>
+    <row r="61" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A61" s="38"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
       <c r="E61" s="38" t="s">
-        <v>668</v>
+        <v>654</v>
       </c>
       <c r="F61" s="38"/>
       <c r="G61" s="38"/>
       <c r="H61" s="38"/>
     </row>
-    <row r="62" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="62" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A62" s="38"/>
       <c r="B62" s="38"/>
       <c r="C62" s="38"/>
       <c r="D62" s="38"/>
       <c r="E62" s="38" t="s">
-        <v>669</v>
+        <v>655</v>
       </c>
       <c r="F62" s="38"/>
       <c r="G62" s="38"/>
       <c r="H62" s="38"/>
     </row>
-    <row r="63" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="63" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A63" s="38"/>
       <c r="B63" s="38"/>
       <c r="C63" s="38"/>
       <c r="D63" s="38"/>
       <c r="E63" s="38" t="s">
-        <v>670</v>
+        <v>656</v>
       </c>
       <c r="F63" s="38"/>
       <c r="G63" s="38"/>
       <c r="H63" s="38"/>
     </row>
-    <row r="64" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="64" spans="1:8" s="39" customFormat="1">
       <c r="A64" s="38"/>
       <c r="B64" s="38"/>
       <c r="C64" s="38"/>
       <c r="D64" s="38"/>
       <c r="E64" s="38" t="s">
-        <v>671</v>
+        <v>657</v>
       </c>
       <c r="F64" s="38"/>
       <c r="G64" s="38"/>
       <c r="H64" s="38"/>
     </row>
-    <row r="65" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="65" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A65" s="38"/>
       <c r="B65" s="38"/>
       <c r="C65" s="38"/>
       <c r="D65" s="38"/>
       <c r="E65" s="38" t="s">
-        <v>672</v>
+        <v>658</v>
       </c>
       <c r="F65" s="38"/>
       <c r="G65" s="38"/>
       <c r="H65" s="38"/>
     </row>
-    <row r="66" spans="1:8" s="39" customFormat="1" ht="29">
+    <row r="66" spans="1:8" s="39" customFormat="1">
       <c r="A66" s="38"/>
       <c r="B66" s="38"/>
       <c r="C66" s="38"/>
       <c r="D66" s="38"/>
       <c r="E66" s="38" t="s">
-        <v>794</v>
+        <v>659</v>
       </c>
       <c r="F66" s="38"/>
       <c r="G66" s="38"/>
       <c r="H66" s="38"/>
     </row>
-    <row r="67" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="67" spans="1:8" s="39" customFormat="1">
       <c r="A67" s="38"/>
       <c r="B67" s="38"/>
       <c r="C67" s="38"/>
       <c r="D67" s="38"/>
       <c r="E67" s="38" t="s">
-        <v>673</v>
+        <v>660</v>
       </c>
       <c r="F67" s="38"/>
       <c r="G67" s="38"/>
       <c r="H67" s="38"/>
     </row>
-    <row r="68" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="68" spans="1:8" s="39" customFormat="1">
       <c r="A68" s="38"/>
       <c r="B68" s="38"/>
       <c r="C68" s="38"/>
       <c r="D68" s="38"/>
       <c r="E68" s="38" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="F68" s="38"/>
       <c r="G68" s="38"/>
       <c r="H68" s="38"/>
     </row>
-    <row r="69" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="69" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A69" s="38"/>
       <c r="B69" s="38"/>
       <c r="C69" s="38"/>
       <c r="D69" s="38"/>
       <c r="E69" s="38" t="s">
-        <v>675</v>
+        <v>662</v>
       </c>
       <c r="F69" s="38"/>
       <c r="G69" s="38"/>
@@ -18790,7 +18863,7 @@
       <c r="C70" s="38"/>
       <c r="D70" s="38"/>
       <c r="E70" s="38" t="s">
-        <v>676</v>
+        <v>663</v>
       </c>
       <c r="F70" s="38"/>
       <c r="G70" s="38"/>
@@ -18802,19 +18875,27 @@
       <c r="C71" s="38"/>
       <c r="D71" s="38"/>
       <c r="E71" s="38" t="s">
-        <v>677</v>
+        <v>664</v>
       </c>
       <c r="F71" s="38"/>
       <c r="G71" s="38"/>
       <c r="H71" s="38"/>
     </row>
-    <row r="72" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
-      <c r="A72" s="38"/>
-      <c r="B72" s="38"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
+    <row r="72" spans="1:8" s="39" customFormat="1" ht="87" customHeight="1">
+      <c r="A72" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="38" t="s">
+        <v>665</v>
+      </c>
+      <c r="C72" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="D72" s="38" t="s">
+        <v>666</v>
+      </c>
       <c r="E72" s="38" t="s">
-        <v>678</v>
+        <v>667</v>
       </c>
       <c r="F72" s="38"/>
       <c r="G72" s="38"/>
@@ -18826,7 +18907,7 @@
       <c r="C73" s="38"/>
       <c r="D73" s="38"/>
       <c r="E73" s="38" t="s">
-        <v>679</v>
+        <v>668</v>
       </c>
       <c r="F73" s="38"/>
       <c r="G73" s="38"/>
@@ -18838,7 +18919,7 @@
       <c r="C74" s="38"/>
       <c r="D74" s="38"/>
       <c r="E74" s="38" t="s">
-        <v>680</v>
+        <v>669</v>
       </c>
       <c r="F74" s="38"/>
       <c r="G74" s="38"/>
@@ -18850,7 +18931,7 @@
       <c r="C75" s="38"/>
       <c r="D75" s="38"/>
       <c r="E75" s="38" t="s">
-        <v>681</v>
+        <v>670</v>
       </c>
       <c r="F75" s="38"/>
       <c r="G75" s="38"/>
@@ -18862,7 +18943,7 @@
       <c r="C76" s="38"/>
       <c r="D76" s="38"/>
       <c r="E76" s="38" t="s">
-        <v>682</v>
+        <v>671</v>
       </c>
       <c r="F76" s="38"/>
       <c r="G76" s="38"/>
@@ -18874,39 +18955,31 @@
       <c r="C77" s="38"/>
       <c r="D77" s="38"/>
       <c r="E77" s="38" t="s">
-        <v>795</v>
+        <v>777</v>
       </c>
       <c r="F77" s="38"/>
       <c r="G77" s="38"/>
       <c r="H77" s="38"/>
     </row>
-    <row r="78" spans="1:8" s="39" customFormat="1" ht="101.5" customHeight="1">
-      <c r="A78" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B78" s="38" t="s">
-        <v>683</v>
-      </c>
-      <c r="C78" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="D78" s="38" t="s">
-        <v>684</v>
-      </c>
+    <row r="78" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A78" s="38"/>
+      <c r="B78" s="38"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="38"/>
       <c r="E78" s="38" t="s">
-        <v>685</v>
+        <v>672</v>
       </c>
       <c r="F78" s="38"/>
       <c r="G78" s="38"/>
       <c r="H78" s="38"/>
     </row>
-    <row r="79" spans="1:8" s="39" customFormat="1">
+    <row r="79" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A79" s="38"/>
       <c r="B79" s="38"/>
       <c r="C79" s="38"/>
       <c r="D79" s="38"/>
       <c r="E79" s="38" t="s">
-        <v>686</v>
+        <v>673</v>
       </c>
       <c r="F79" s="38"/>
       <c r="G79" s="38"/>
@@ -18918,19 +18991,19 @@
       <c r="C80" s="38"/>
       <c r="D80" s="38"/>
       <c r="E80" s="38" t="s">
-        <v>687</v>
+        <v>674</v>
       </c>
       <c r="F80" s="38"/>
       <c r="G80" s="38"/>
       <c r="H80" s="38"/>
     </row>
-    <row r="81" spans="1:8" s="39" customFormat="1">
+    <row r="81" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A81" s="38"/>
       <c r="B81" s="38"/>
       <c r="C81" s="38"/>
       <c r="D81" s="38"/>
       <c r="E81" s="38" t="s">
-        <v>688</v>
+        <v>675</v>
       </c>
       <c r="F81" s="38"/>
       <c r="G81" s="38"/>
@@ -18942,7 +19015,7 @@
       <c r="C82" s="38"/>
       <c r="D82" s="38"/>
       <c r="E82" s="38" t="s">
-        <v>689</v>
+        <v>676</v>
       </c>
       <c r="F82" s="38"/>
       <c r="G82" s="38"/>
@@ -18954,7 +19027,7 @@
       <c r="C83" s="38"/>
       <c r="D83" s="38"/>
       <c r="E83" s="38" t="s">
-        <v>690</v>
+        <v>677</v>
       </c>
       <c r="F83" s="38"/>
       <c r="G83" s="38"/>
@@ -18966,7 +19039,7 @@
       <c r="C84" s="38"/>
       <c r="D84" s="38"/>
       <c r="E84" s="38" t="s">
-        <v>691</v>
+        <v>678</v>
       </c>
       <c r="F84" s="38"/>
       <c r="G84" s="38"/>
@@ -18978,7 +19051,7 @@
       <c r="C85" s="38"/>
       <c r="D85" s="38"/>
       <c r="E85" s="38" t="s">
-        <v>692</v>
+        <v>679</v>
       </c>
       <c r="F85" s="38"/>
       <c r="G85" s="38"/>
@@ -18990,7 +19063,7 @@
       <c r="C86" s="38"/>
       <c r="D86" s="38"/>
       <c r="E86" s="38" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
       <c r="F86" s="38"/>
       <c r="G86" s="38"/>
@@ -19002,7 +19075,7 @@
       <c r="C87" s="38"/>
       <c r="D87" s="38"/>
       <c r="E87" s="38" t="s">
-        <v>694</v>
+        <v>681</v>
       </c>
       <c r="F87" s="38"/>
       <c r="G87" s="38"/>
@@ -19014,19 +19087,19 @@
       <c r="C88" s="38"/>
       <c r="D88" s="38"/>
       <c r="E88" s="38" t="s">
-        <v>695</v>
+        <v>778</v>
       </c>
       <c r="F88" s="38"/>
       <c r="G88" s="38"/>
       <c r="H88" s="38"/>
     </row>
-    <row r="89" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="89" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A89" s="38"/>
       <c r="B89" s="38"/>
       <c r="C89" s="38"/>
       <c r="D89" s="38"/>
       <c r="E89" s="38" t="s">
-        <v>696</v>
+        <v>907</v>
       </c>
       <c r="F89" s="38"/>
       <c r="G89" s="38"/>
@@ -19038,31 +19111,39 @@
       <c r="C90" s="38"/>
       <c r="D90" s="38"/>
       <c r="E90" s="38" t="s">
-        <v>697</v>
+        <v>892</v>
       </c>
       <c r="F90" s="38"/>
       <c r="G90" s="38"/>
       <c r="H90" s="38"/>
     </row>
-    <row r="91" spans="1:8" s="39" customFormat="1" ht="29">
-      <c r="A91" s="38"/>
-      <c r="B91" s="38"/>
-      <c r="C91" s="38"/>
-      <c r="D91" s="38"/>
+    <row r="91" spans="1:8" s="39" customFormat="1" ht="101.5" customHeight="1">
+      <c r="A91" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" s="38" t="s">
+        <v>682</v>
+      </c>
+      <c r="C91" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="D91" s="38" t="s">
+        <v>683</v>
+      </c>
       <c r="E91" s="38" t="s">
-        <v>698</v>
+        <v>893</v>
       </c>
       <c r="F91" s="38"/>
       <c r="G91" s="38"/>
       <c r="H91" s="38"/>
     </row>
-    <row r="92" spans="1:8" s="39" customFormat="1">
+    <row r="92" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A92" s="38"/>
       <c r="B92" s="38"/>
       <c r="C92" s="38"/>
       <c r="D92" s="38"/>
       <c r="E92" s="38" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="F92" s="38"/>
       <c r="G92" s="38"/>
@@ -19074,39 +19155,31 @@
       <c r="C93" s="38"/>
       <c r="D93" s="38"/>
       <c r="E93" s="38" t="s">
-        <v>700</v>
+        <v>689</v>
       </c>
       <c r="F93" s="38"/>
       <c r="G93" s="38"/>
       <c r="H93" s="38"/>
     </row>
-    <row r="94" spans="1:8" s="39" customFormat="1">
+    <row r="94" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A94" s="38"/>
       <c r="B94" s="38"/>
       <c r="C94" s="38"/>
       <c r="D94" s="38"/>
       <c r="E94" s="38" t="s">
-        <v>796</v>
+        <v>690</v>
       </c>
       <c r="F94" s="38"/>
       <c r="G94" s="38"/>
       <c r="H94" s="38"/>
     </row>
-    <row r="95" spans="1:8" s="39" customFormat="1" ht="101.5" customHeight="1">
-      <c r="A95" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B95" s="38" t="s">
-        <v>701</v>
-      </c>
-      <c r="C95" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="D95" s="38" t="s">
-        <v>702</v>
-      </c>
+    <row r="95" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A95" s="38"/>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="38"/>
       <c r="E95" s="38" t="s">
-        <v>703</v>
+        <v>691</v>
       </c>
       <c r="F95" s="38"/>
       <c r="G95" s="38"/>
@@ -19118,7 +19191,7 @@
       <c r="C96" s="38"/>
       <c r="D96" s="38"/>
       <c r="E96" s="38" t="s">
-        <v>704</v>
+        <v>692</v>
       </c>
       <c r="F96" s="38"/>
       <c r="G96" s="38"/>
@@ -19130,7 +19203,7 @@
       <c r="C97" s="38"/>
       <c r="D97" s="38"/>
       <c r="E97" s="38" t="s">
-        <v>705</v>
+        <v>693</v>
       </c>
       <c r="F97" s="38"/>
       <c r="G97" s="38"/>
@@ -19142,7 +19215,7 @@
       <c r="C98" s="38"/>
       <c r="D98" s="38"/>
       <c r="E98" s="38" t="s">
-        <v>706</v>
+        <v>894</v>
       </c>
       <c r="F98" s="38"/>
       <c r="G98" s="38"/>
@@ -19154,7 +19227,7 @@
       <c r="C99" s="38"/>
       <c r="D99" s="38"/>
       <c r="E99" s="38" t="s">
-        <v>707</v>
+        <v>684</v>
       </c>
       <c r="F99" s="38"/>
       <c r="G99" s="38"/>
@@ -19166,19 +19239,19 @@
       <c r="C100" s="38"/>
       <c r="D100" s="38"/>
       <c r="E100" s="38" t="s">
-        <v>708</v>
+        <v>895</v>
       </c>
       <c r="F100" s="38"/>
       <c r="G100" s="38"/>
       <c r="H100" s="38"/>
     </row>
-    <row r="101" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="101" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A101" s="38"/>
       <c r="B101" s="38"/>
       <c r="C101" s="38"/>
       <c r="D101" s="38"/>
       <c r="E101" s="38" t="s">
-        <v>709</v>
+        <v>896</v>
       </c>
       <c r="F101" s="38"/>
       <c r="G101" s="38"/>
@@ -19190,19 +19263,19 @@
       <c r="C102" s="38"/>
       <c r="D102" s="38"/>
       <c r="E102" s="38" t="s">
-        <v>710</v>
+        <v>897</v>
       </c>
       <c r="F102" s="38"/>
       <c r="G102" s="38"/>
       <c r="H102" s="38"/>
     </row>
-    <row r="103" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="103" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A103" s="38"/>
       <c r="B103" s="38"/>
       <c r="C103" s="38"/>
       <c r="D103" s="38"/>
       <c r="E103" s="38" t="s">
-        <v>711</v>
+        <v>685</v>
       </c>
       <c r="F103" s="38"/>
       <c r="G103" s="38"/>
@@ -19214,83 +19287,75 @@
       <c r="C104" s="38"/>
       <c r="D104" s="38"/>
       <c r="E104" s="38" t="s">
-        <v>797</v>
+        <v>687</v>
       </c>
       <c r="F104" s="38"/>
       <c r="G104" s="38"/>
       <c r="H104" s="38"/>
     </row>
-    <row r="105" spans="1:8" s="39" customFormat="1" ht="72.5">
-      <c r="A105" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B105" s="38" t="s">
-        <v>800</v>
-      </c>
-      <c r="C105" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="D105" s="38" t="s">
-        <v>798</v>
-      </c>
+    <row r="105" spans="1:8" s="39" customFormat="1" ht="29">
+      <c r="A105" s="38"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="38"/>
       <c r="E105" s="38" t="s">
-        <v>799</v>
+        <v>688</v>
       </c>
       <c r="F105" s="38"/>
       <c r="G105" s="38"/>
       <c r="H105" s="38"/>
     </row>
-    <row r="106" spans="1:8" s="39" customFormat="1" ht="101.5" customHeight="1">
-      <c r="A106" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B106" s="38" t="s">
-        <v>712</v>
-      </c>
-      <c r="C106" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="D106" s="38" t="s">
-        <v>713</v>
-      </c>
+    <row r="106" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A106" s="38"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="38"/>
+      <c r="D106" s="38"/>
       <c r="E106" s="38" t="s">
-        <v>714</v>
+        <v>898</v>
       </c>
       <c r="F106" s="38"/>
       <c r="G106" s="38"/>
       <c r="H106" s="38"/>
     </row>
-    <row r="107" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="107" spans="1:8" s="39" customFormat="1">
       <c r="A107" s="38"/>
       <c r="B107" s="38"/>
       <c r="C107" s="38"/>
       <c r="D107" s="38"/>
       <c r="E107" s="38" t="s">
-        <v>715</v>
+        <v>899</v>
       </c>
       <c r="F107" s="38"/>
       <c r="G107" s="38"/>
       <c r="H107" s="38"/>
     </row>
-    <row r="108" spans="1:8" s="39" customFormat="1" ht="43.5" customHeight="1">
+    <row r="108" spans="1:8" s="39" customFormat="1">
       <c r="A108" s="38"/>
       <c r="B108" s="38"/>
       <c r="C108" s="38"/>
       <c r="D108" s="38"/>
       <c r="E108" s="38" t="s">
-        <v>716</v>
+        <v>900</v>
       </c>
       <c r="F108" s="38"/>
       <c r="G108" s="38"/>
       <c r="H108" s="38"/>
     </row>
-    <row r="109" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
-      <c r="A109" s="38"/>
-      <c r="B109" s="38"/>
-      <c r="C109" s="38"/>
-      <c r="D109" s="38"/>
+    <row r="109" spans="1:8" s="39" customFormat="1" ht="101.5" customHeight="1">
+      <c r="A109" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" s="38" t="s">
+        <v>694</v>
+      </c>
+      <c r="C109" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="D109" s="38" t="s">
+        <v>695</v>
+      </c>
       <c r="E109" s="38" t="s">
-        <v>717</v>
+        <v>696</v>
       </c>
       <c r="F109" s="38"/>
       <c r="G109" s="38"/>
@@ -19302,7 +19367,7 @@
       <c r="C110" s="38"/>
       <c r="D110" s="38"/>
       <c r="E110" s="38" t="s">
-        <v>718</v>
+        <v>697</v>
       </c>
       <c r="F110" s="38"/>
       <c r="G110" s="38"/>
@@ -19314,7 +19379,7 @@
       <c r="C111" s="38"/>
       <c r="D111" s="38"/>
       <c r="E111" s="38" t="s">
-        <v>719</v>
+        <v>698</v>
       </c>
       <c r="F111" s="38"/>
       <c r="G111" s="38"/>
@@ -19326,7 +19391,7 @@
       <c r="C112" s="38"/>
       <c r="D112" s="38"/>
       <c r="E112" s="38" t="s">
-        <v>720</v>
+        <v>699</v>
       </c>
       <c r="F112" s="38"/>
       <c r="G112" s="38"/>
@@ -19338,7 +19403,7 @@
       <c r="C113" s="38"/>
       <c r="D113" s="38"/>
       <c r="E113" s="38" t="s">
-        <v>721</v>
+        <v>700</v>
       </c>
       <c r="F113" s="38"/>
       <c r="G113" s="38"/>
@@ -19350,7 +19415,7 @@
       <c r="C114" s="38"/>
       <c r="D114" s="38"/>
       <c r="E114" s="38" t="s">
-        <v>722</v>
+        <v>701</v>
       </c>
       <c r="F114" s="38"/>
       <c r="G114" s="38"/>
@@ -19362,7 +19427,7 @@
       <c r="C115" s="38"/>
       <c r="D115" s="38"/>
       <c r="E115" s="38" t="s">
-        <v>723</v>
+        <v>702</v>
       </c>
       <c r="F115" s="38"/>
       <c r="G115" s="38"/>
@@ -19374,7 +19439,7 @@
       <c r="C116" s="38"/>
       <c r="D116" s="38"/>
       <c r="E116" s="38" t="s">
-        <v>724</v>
+        <v>703</v>
       </c>
       <c r="F116" s="38"/>
       <c r="G116" s="38"/>
@@ -19386,67 +19451,83 @@
       <c r="C117" s="38"/>
       <c r="D117" s="38"/>
       <c r="E117" s="38" t="s">
-        <v>725</v>
+        <v>704</v>
       </c>
       <c r="F117" s="38"/>
       <c r="G117" s="38"/>
       <c r="H117" s="38"/>
     </row>
-    <row r="118" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="118" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A118" s="38"/>
       <c r="B118" s="38"/>
       <c r="C118" s="38"/>
       <c r="D118" s="38"/>
       <c r="E118" s="38" t="s">
-        <v>726</v>
+        <v>779</v>
       </c>
       <c r="F118" s="38"/>
       <c r="G118" s="38"/>
       <c r="H118" s="38"/>
     </row>
-    <row r="119" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="119" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A119" s="38"/>
       <c r="B119" s="38"/>
       <c r="C119" s="38"/>
       <c r="D119" s="38"/>
       <c r="E119" s="38" t="s">
-        <v>727</v>
+        <v>906</v>
       </c>
       <c r="F119" s="38"/>
       <c r="G119" s="38"/>
       <c r="H119" s="38"/>
     </row>
-    <row r="120" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="120" spans="1:8" s="39" customFormat="1" ht="29">
       <c r="A120" s="38"/>
       <c r="B120" s="38"/>
       <c r="C120" s="38"/>
       <c r="D120" s="38"/>
       <c r="E120" s="38" t="s">
-        <v>728</v>
+        <v>901</v>
       </c>
       <c r="F120" s="38"/>
       <c r="G120" s="38"/>
       <c r="H120" s="38"/>
     </row>
-    <row r="121" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
-      <c r="A121" s="38"/>
-      <c r="B121" s="38"/>
-      <c r="C121" s="38"/>
-      <c r="D121" s="38"/>
+    <row r="121" spans="1:8" s="39" customFormat="1" ht="72.5">
+      <c r="A121" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121" s="38" t="s">
+        <v>782</v>
+      </c>
+      <c r="C121" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="D121" s="38" t="s">
+        <v>780</v>
+      </c>
       <c r="E121" s="38" t="s">
-        <v>729</v>
+        <v>781</v>
       </c>
       <c r="F121" s="38"/>
       <c r="G121" s="38"/>
       <c r="H121" s="38"/>
     </row>
-    <row r="122" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
-      <c r="A122" s="38"/>
-      <c r="B122" s="38"/>
-      <c r="C122" s="38"/>
-      <c r="D122" s="38"/>
+    <row r="122" spans="1:8" s="39" customFormat="1" ht="101.5" customHeight="1">
+      <c r="A122" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B122" s="93" t="s">
+        <v>705</v>
+      </c>
+      <c r="C122" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="D122" s="38" t="s">
+        <v>706</v>
+      </c>
       <c r="E122" s="38" t="s">
-        <v>730</v>
+        <v>719</v>
       </c>
       <c r="F122" s="38"/>
       <c r="G122" s="38"/>
@@ -19458,19 +19539,19 @@
       <c r="C123" s="38"/>
       <c r="D123" s="38"/>
       <c r="E123" s="38" t="s">
-        <v>731</v>
+        <v>720</v>
       </c>
       <c r="F123" s="38"/>
       <c r="G123" s="38"/>
       <c r="H123" s="38"/>
     </row>
-    <row r="124" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+    <row r="124" spans="1:8" s="39" customFormat="1" ht="43.5" customHeight="1">
       <c r="A124" s="38"/>
       <c r="B124" s="38"/>
       <c r="C124" s="38"/>
       <c r="D124" s="38"/>
       <c r="E124" s="38" t="s">
-        <v>732</v>
+        <v>902</v>
       </c>
       <c r="F124" s="38"/>
       <c r="G124" s="38"/>
@@ -19482,7 +19563,7 @@
       <c r="C125" s="38"/>
       <c r="D125" s="38"/>
       <c r="E125" s="38" t="s">
-        <v>733</v>
+        <v>722</v>
       </c>
       <c r="F125" s="38"/>
       <c r="G125" s="38"/>
@@ -19494,7 +19575,7 @@
       <c r="C126" s="38"/>
       <c r="D126" s="38"/>
       <c r="E126" s="38" t="s">
-        <v>734</v>
+        <v>725</v>
       </c>
       <c r="F126" s="38"/>
       <c r="G126" s="38"/>
@@ -19506,31 +19587,31 @@
       <c r="C127" s="38"/>
       <c r="D127" s="38"/>
       <c r="E127" s="38" t="s">
-        <v>735</v>
+        <v>726</v>
       </c>
       <c r="F127" s="38"/>
       <c r="G127" s="38"/>
       <c r="H127" s="38"/>
     </row>
-    <row r="128" spans="1:8" s="39" customFormat="1" ht="29">
+    <row r="128" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A128" s="38"/>
       <c r="B128" s="38"/>
       <c r="C128" s="38"/>
       <c r="D128" s="38"/>
       <c r="E128" s="38" t="s">
-        <v>736</v>
+        <v>727</v>
       </c>
       <c r="F128" s="38"/>
       <c r="G128" s="38"/>
       <c r="H128" s="38"/>
     </row>
-    <row r="129" spans="1:8" s="39" customFormat="1">
+    <row r="129" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A129" s="38"/>
       <c r="B129" s="38"/>
       <c r="C129" s="38"/>
       <c r="D129" s="38"/>
       <c r="E129" s="38" t="s">
-        <v>737</v>
+        <v>707</v>
       </c>
       <c r="F129" s="38"/>
       <c r="G129" s="38"/>
@@ -19542,7 +19623,7 @@
       <c r="C130" s="38"/>
       <c r="D130" s="38"/>
       <c r="E130" s="38" t="s">
-        <v>738</v>
+        <v>708</v>
       </c>
       <c r="F130" s="38"/>
       <c r="G130" s="38"/>
@@ -19554,7 +19635,7 @@
       <c r="C131" s="38"/>
       <c r="D131" s="38"/>
       <c r="E131" s="38" t="s">
-        <v>739</v>
+        <v>709</v>
       </c>
       <c r="F131" s="38"/>
       <c r="G131" s="38"/>
@@ -19566,19 +19647,19 @@
       <c r="C132" s="38"/>
       <c r="D132" s="38"/>
       <c r="E132" s="38" t="s">
-        <v>740</v>
+        <v>710</v>
       </c>
       <c r="F132" s="38"/>
       <c r="G132" s="38"/>
       <c r="H132" s="38"/>
     </row>
-    <row r="133" spans="1:8" s="39" customFormat="1">
+    <row r="133" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
       <c r="A133" s="38"/>
       <c r="B133" s="38"/>
       <c r="C133" s="38"/>
       <c r="D133" s="38"/>
       <c r="E133" s="38" t="s">
-        <v>741</v>
+        <v>711</v>
       </c>
       <c r="F133" s="38"/>
       <c r="G133" s="38"/>
@@ -19590,7 +19671,7 @@
       <c r="C134" s="38"/>
       <c r="D134" s="38"/>
       <c r="E134" s="38" t="s">
-        <v>742</v>
+        <v>712</v>
       </c>
       <c r="F134" s="38"/>
       <c r="G134" s="38"/>
@@ -19602,7 +19683,7 @@
       <c r="C135" s="38"/>
       <c r="D135" s="38"/>
       <c r="E135" s="38" t="s">
-        <v>743</v>
+        <v>713</v>
       </c>
       <c r="F135" s="38"/>
       <c r="G135" s="38"/>
@@ -19614,31 +19695,225 @@
       <c r="C136" s="38"/>
       <c r="D136" s="38"/>
       <c r="E136" s="38" t="s">
-        <v>744</v>
+        <v>714</v>
       </c>
       <c r="F136" s="38"/>
       <c r="G136" s="38"/>
       <c r="H136" s="38"/>
     </row>
-    <row r="137" spans="1:8" s="39" customFormat="1" ht="43.5" customHeight="1">
-      <c r="A137" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B137" s="38" t="s">
-        <v>745</v>
-      </c>
-      <c r="C137" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="D137" s="38" t="s">
-        <v>746</v>
-      </c>
+    <row r="137" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A137" s="38"/>
+      <c r="B137" s="38"/>
+      <c r="C137" s="38"/>
+      <c r="D137" s="38"/>
       <c r="E137" s="38" t="s">
-        <v>747</v>
+        <v>715</v>
       </c>
       <c r="F137" s="38"/>
       <c r="G137" s="38"/>
       <c r="H137" s="38"/>
+    </row>
+    <row r="138" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A138" s="38"/>
+      <c r="B138" s="38"/>
+      <c r="C138" s="38"/>
+      <c r="D138" s="38"/>
+      <c r="E138" s="38" t="s">
+        <v>716</v>
+      </c>
+      <c r="F138" s="38"/>
+      <c r="G138" s="38"/>
+      <c r="H138" s="38"/>
+    </row>
+    <row r="139" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A139" s="38"/>
+      <c r="B139" s="38"/>
+      <c r="C139" s="38"/>
+      <c r="D139" s="38"/>
+      <c r="E139" s="38" t="s">
+        <v>717</v>
+      </c>
+      <c r="F139" s="38"/>
+      <c r="G139" s="38"/>
+      <c r="H139" s="38"/>
+    </row>
+    <row r="140" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A140" s="38"/>
+      <c r="B140" s="38"/>
+      <c r="C140" s="38"/>
+      <c r="D140" s="38"/>
+      <c r="E140" s="38" t="s">
+        <v>718</v>
+      </c>
+      <c r="F140" s="38"/>
+      <c r="G140" s="38"/>
+      <c r="H140" s="38"/>
+    </row>
+    <row r="141" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A141" s="38"/>
+      <c r="B141" s="38"/>
+      <c r="C141" s="38"/>
+      <c r="D141" s="38"/>
+      <c r="E141" s="38" t="s">
+        <v>908</v>
+      </c>
+      <c r="F141" s="38"/>
+      <c r="G141" s="38"/>
+      <c r="H141" s="38"/>
+    </row>
+    <row r="142" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A142" s="38"/>
+      <c r="B142" s="38"/>
+      <c r="C142" s="38"/>
+      <c r="D142" s="38"/>
+      <c r="E142" s="38" t="s">
+        <v>909</v>
+      </c>
+      <c r="F142" s="38"/>
+      <c r="G142" s="38"/>
+      <c r="H142" s="38"/>
+    </row>
+    <row r="143" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A143" s="38"/>
+      <c r="B143" s="38"/>
+      <c r="C143" s="38"/>
+      <c r="D143" s="38"/>
+      <c r="E143" s="38" t="s">
+        <v>910</v>
+      </c>
+      <c r="F143" s="38"/>
+      <c r="G143" s="38"/>
+      <c r="H143" s="38"/>
+    </row>
+    <row r="144" spans="1:8" s="39" customFormat="1" ht="29">
+      <c r="A144" s="38"/>
+      <c r="B144" s="38"/>
+      <c r="C144" s="38"/>
+      <c r="D144" s="38"/>
+      <c r="E144" s="38" t="s">
+        <v>911</v>
+      </c>
+      <c r="F144" s="38"/>
+      <c r="G144" s="38"/>
+      <c r="H144" s="38"/>
+    </row>
+    <row r="145" spans="1:8" s="39" customFormat="1" ht="29">
+      <c r="A145" s="38"/>
+      <c r="B145" s="38"/>
+      <c r="C145" s="38"/>
+      <c r="D145" s="38"/>
+      <c r="E145" s="38" t="s">
+        <v>728</v>
+      </c>
+      <c r="F145" s="38"/>
+      <c r="G145" s="38"/>
+      <c r="H145" s="38"/>
+    </row>
+    <row r="146" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A146" s="38"/>
+      <c r="B146" s="38"/>
+      <c r="C146" s="38"/>
+      <c r="D146" s="38"/>
+      <c r="E146" s="38" t="s">
+        <v>729</v>
+      </c>
+      <c r="F146" s="38"/>
+      <c r="G146" s="38"/>
+      <c r="H146" s="38"/>
+    </row>
+    <row r="147" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A147" s="38"/>
+      <c r="B147" s="38"/>
+      <c r="C147" s="38"/>
+      <c r="D147" s="38"/>
+      <c r="E147" s="38" t="s">
+        <v>730</v>
+      </c>
+      <c r="F147" s="38"/>
+      <c r="G147" s="38"/>
+      <c r="H147" s="38"/>
+    </row>
+    <row r="148" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A148" s="38"/>
+      <c r="B148" s="38"/>
+      <c r="C148" s="38"/>
+      <c r="D148" s="38"/>
+      <c r="E148" s="38" t="s">
+        <v>905</v>
+      </c>
+      <c r="F148" s="38"/>
+      <c r="G148" s="38"/>
+      <c r="H148" s="38"/>
+    </row>
+    <row r="149" spans="1:8" s="39" customFormat="1" ht="29">
+      <c r="A149" s="38"/>
+      <c r="B149" s="38"/>
+      <c r="C149" s="38"/>
+      <c r="D149" s="38"/>
+      <c r="E149" s="38" t="s">
+        <v>903</v>
+      </c>
+      <c r="F149" s="38"/>
+      <c r="G149" s="38"/>
+      <c r="H149" s="38"/>
+    </row>
+    <row r="150" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A150" s="38"/>
+      <c r="B150" s="38"/>
+      <c r="C150" s="38"/>
+      <c r="D150" s="38"/>
+      <c r="E150" s="38" t="s">
+        <v>721</v>
+      </c>
+      <c r="F150" s="38"/>
+      <c r="G150" s="38"/>
+      <c r="H150" s="38"/>
+    </row>
+    <row r="151" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A151" s="38"/>
+      <c r="B151" s="38"/>
+      <c r="C151" s="38"/>
+      <c r="D151" s="38"/>
+      <c r="E151" s="38" t="s">
+        <v>723</v>
+      </c>
+      <c r="F151" s="38"/>
+      <c r="G151" s="38"/>
+      <c r="H151" s="38"/>
+    </row>
+    <row r="152" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A152" s="38"/>
+      <c r="B152" s="38"/>
+      <c r="C152" s="38"/>
+      <c r="D152" s="38"/>
+      <c r="E152" s="38" t="s">
+        <v>724</v>
+      </c>
+      <c r="F152" s="38"/>
+      <c r="G152" s="38"/>
+      <c r="H152" s="38"/>
+    </row>
+    <row r="153" spans="1:8" s="39" customFormat="1" ht="29" customHeight="1">
+      <c r="A153" s="38"/>
+      <c r="B153" s="38"/>
+      <c r="C153" s="38"/>
+      <c r="D153" s="38"/>
+      <c r="E153" s="38" t="s">
+        <v>904</v>
+      </c>
+      <c r="F153" s="38"/>
+      <c r="G153" s="38"/>
+      <c r="H153" s="38"/>
+    </row>
+    <row r="154" spans="1:8" s="39" customFormat="1" ht="60" customHeight="1">
+      <c r="A154" s="38"/>
+      <c r="B154" s="38"/>
+      <c r="C154" s="38"/>
+      <c r="D154" s="38"/>
+      <c r="E154" s="38"/>
+      <c r="F154" s="38"/>
+      <c r="G154" s="38"/>
+      <c r="H154" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -19671,20 +19946,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="131.5" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>477</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="96" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="98" t="s">
         <v>476</v>
       </c>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="98"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="100"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="44" t="s">
@@ -19726,16 +20001,16 @@
         <v>406</v>
       </c>
       <c r="C3" s="69" t="s">
-        <v>812</v>
+        <v>794</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>807</v>
+        <v>789</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>801</v>
+        <v>783</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>802</v>
+        <v>784</v>
       </c>
       <c r="G3" s="38" t="b">
         <v>1</v>
@@ -19745,7 +20020,7 @@
         <v>406</v>
       </c>
       <c r="J3" s="38" t="s">
-        <v>803</v>
+        <v>785</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="39" customFormat="1" ht="29">
@@ -19756,16 +20031,16 @@
         <v>406</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>812</v>
+        <v>794</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>807</v>
+        <v>789</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>804</v>
+        <v>786</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>805</v>
+        <v>787</v>
       </c>
       <c r="G4" s="38" t="b">
         <v>0</v>
@@ -19775,7 +20050,7 @@
         <v>406</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>806</v>
+        <v>788</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -20050,22 +20325,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="39" customFormat="1" ht="187.75" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>463</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="93" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="95" t="s">
         <v>464</v>
       </c>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="95"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="97"/>
     </row>
     <row r="2" spans="1:12" s="47" customFormat="1" ht="45" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -20113,13 +20388,13 @@
         <v>355</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>885</v>
+        <v>867</v>
       </c>
       <c r="F3" s="40" t="s">
         <v>21</v>
@@ -20134,7 +20409,7 @@
         <v>24</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>767</v>
+        <v>750</v>
       </c>
       <c r="K3" s="40"/>
       <c r="L3" s="34"/>
@@ -20293,17 +20568,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="221" customHeight="1">
-      <c r="A1" s="93" t="s">
-        <v>892</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="93" t="s">
-        <v>893</v>
-      </c>
-      <c r="G1" s="94"/>
+      <c r="A1" s="95" t="s">
+        <v>874</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="95" t="s">
+        <v>875</v>
+      </c>
+      <c r="G1" s="96"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="89" t="s">
@@ -20313,19 +20588,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="89" t="s">
-        <v>878</v>
+        <v>860</v>
       </c>
       <c r="D2" s="89" t="s">
-        <v>879</v>
+        <v>861</v>
       </c>
       <c r="E2" s="89" t="s">
-        <v>880</v>
+        <v>862</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>881</v>
+        <v>863</v>
       </c>
       <c r="G2" s="91" t="s">
-        <v>882</v>
+        <v>864</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" customHeight="1">
@@ -20336,19 +20611,19 @@
         <v>355</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>885</v>
+        <v>867</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>886</v>
+        <v>868</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>887</v>
+        <v>869</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>888</v>
+        <v>870</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>889</v>
+        <v>871</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="94.5" customHeight="1">
@@ -20621,10 +20896,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="47" customFormat="1" ht="121.75" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>443</v>
       </c>
-      <c r="B1" s="98"/>
+      <c r="B1" s="100"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="11" t="s">
@@ -20694,16 +20969,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="103.75" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>450</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
     </row>
     <row r="2" spans="1:8" s="47" customFormat="1" ht="43.25" customHeight="1">
       <c r="A2" s="11" t="s">
@@ -20739,7 +21014,7 @@
         <v>355</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>38</v>
@@ -20748,7 +21023,7 @@
         <v>41</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>811</v>
+        <v>793</v>
       </c>
       <c r="G3" s="40"/>
       <c r="H3" s="40"/>

</xml_diff>